<commit_message>
ajustando quantitativo de câmeras.
</commit_message>
<xml_diff>
--- a/data/Prioridades.xlsx
+++ b/data/Prioridades.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Consultor\OneDrive - Aquila\Área de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Consultor\Desktop\COP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86E76D2-A606-444F-813D-C55433335D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B31728-6FD3-4FD7-A271-B4FA3228001B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{397ABB56-F0FE-4E29-B5CB-823307B18FC8}"/>
   </bookViews>
@@ -727,10 +727,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
-    <numFmt numFmtId="169" formatCode="#,##0.000000"/>
-    <numFmt numFmtId="177" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -771,6 +771,14 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -863,20 +871,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="177" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1194,7 +1202,7 @@
   <dimension ref="A1:G676"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1214,7 +1222,7 @@
       <c r="B1" t="s">
         <v>116</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="25" t="s">
         <v>0</v>
       </c>
       <c r="D1" t="s">
@@ -1471,7 +1479,7 @@
       <c r="A14" t="s">
         <v>128</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" t="s">
         <v>123</v>
       </c>
       <c r="C14">
@@ -3694,11 +3702,14 @@
       <c r="B125" s="22" t="s">
         <v>225</v>
       </c>
-      <c r="C125" s="24">
+      <c r="C125" s="23">
         <v>-8.0635997672068793</v>
       </c>
-      <c r="D125" s="24">
+      <c r="D125" s="23">
         <v>-34.881890011734797</v>
+      </c>
+      <c r="F125" s="22">
+        <v>6</v>
       </c>
     </row>
     <row r="126" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
@@ -3708,10 +3719,10 @@
       <c r="B126" s="22" t="s">
         <v>226</v>
       </c>
-      <c r="C126" s="25">
+      <c r="C126" s="24">
         <v>-8.0297949481864208</v>
       </c>
-      <c r="D126" s="25">
+      <c r="D126" s="24">
         <v>-34.929545690228501</v>
       </c>
     </row>
@@ -4486,7 +4497,6 @@
       <c r="D676" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F141" xr:uid="{22014C47-1C13-4AB1-9850-A592523522E1}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>

<commit_message>
acrescentando dados de CVP, aviso de cobertura e atualizando pontos mínimos.
</commit_message>
<xml_diff>
--- a/data/Prioridades.xlsx
+++ b/data/Prioridades.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Consultor\Desktop\COP\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Consultor\OneDrive - Aquila\Área de Trabalho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51B31728-6FD3-4FD7-A271-B4FA3228001B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8860369-639D-4094-95A9-2076E546D450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{397ABB56-F0FE-4E29-B5CB-823307B18FC8}"/>
   </bookViews>
@@ -38,13 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="227">
-  <si>
-    <t>LATITUDE COM PONTO</t>
-  </si>
-  <si>
-    <t>LONGITUDE COM PONTO</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="227">
   <si>
     <t>AVENIDA CAXANGA</t>
   </si>
@@ -719,6 +713,12 @@
   </si>
   <si>
     <t>Ponte Engenheiro jaime Gusmão</t>
+  </si>
+  <si>
+    <t>lat</t>
+  </si>
+  <si>
+    <t>log</t>
   </si>
 </sst>
 </file>
@@ -753,14 +753,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="4" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -773,9 +765,15 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="7"/>
+      <color rgb="FF007B8B"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="4" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -840,7 +838,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -858,33 +856,36 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1202,7 +1203,7 @@
   <dimension ref="A1:G676"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F134" sqref="F134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1217,55 +1218,55 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D1" t="s">
+        <v>226</v>
+      </c>
+      <c r="E1" t="s">
         <v>115</v>
       </c>
-      <c r="B1" t="s">
+      <c r="F1" t="s">
         <v>116</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>117</v>
-      </c>
-      <c r="F1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>121</v>
-      </c>
-      <c r="C2">
+        <v>119</v>
+      </c>
+      <c r="C2" s="13">
         <v>-8.0625199999999992</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="13">
         <v>-34.931939999999997</v>
       </c>
       <c r="E2">
         <v>7</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="C3">
+        <v>134</v>
+      </c>
+      <c r="C3" s="13">
         <v>-8.0349699999999995</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="13">
         <v>-34.949379999999998</v>
       </c>
       <c r="E3">
@@ -1277,15 +1278,15 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4">
+        <v>124</v>
+      </c>
+      <c r="C4" s="13">
         <v>-8.0387400000000007</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="13">
         <v>-34.942459999999997</v>
       </c>
       <c r="E4">
@@ -1297,15 +1298,15 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="C5">
+        <v>135</v>
+      </c>
+      <c r="C5" s="13">
         <v>-8.0782500000000006</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="13">
         <v>-34.909379999999999</v>
       </c>
       <c r="E5">
@@ -1317,15 +1318,15 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="C6">
+        <v>137</v>
+      </c>
+      <c r="C6" s="13">
         <v>-8.0895499999999991</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="13">
         <v>-34.882910000000003</v>
       </c>
       <c r="E6">
@@ -1337,15 +1338,15 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="C7">
+        <v>140</v>
+      </c>
+      <c r="C7" s="13">
         <v>-8.11951</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="13">
         <v>-34.896729999999998</v>
       </c>
       <c r="E7">
@@ -1357,15 +1358,15 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="C8">
+        <v>130</v>
+      </c>
+      <c r="C8" s="13">
         <v>-8.0474399999999999</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="13">
         <v>-34.876989999999999</v>
       </c>
       <c r="E8">
@@ -1377,15 +1378,15 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
-      </c>
-      <c r="C9">
+        <v>129</v>
+      </c>
+      <c r="C9" s="13">
         <v>-8.0848800000000001</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="13">
         <v>-34.928669999999997</v>
       </c>
       <c r="E9">
@@ -1397,15 +1398,15 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B10" t="s">
-        <v>123</v>
-      </c>
-      <c r="C10">
+        <v>121</v>
+      </c>
+      <c r="C10" s="13">
         <v>-8.1367899999999995</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="13">
         <v>-34.916919999999998</v>
       </c>
       <c r="E10">
@@ -1417,35 +1418,35 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B11" t="s">
-        <v>123</v>
-      </c>
-      <c r="C11">
+        <v>121</v>
+      </c>
+      <c r="C11" s="13">
         <v>-8.1222300000000001</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="13">
         <v>-34.914400000000001</v>
       </c>
       <c r="E11">
         <v>35</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B12" t="s">
-        <v>123</v>
-      </c>
-      <c r="C12">
+        <v>121</v>
+      </c>
+      <c r="C12" s="13">
         <v>-8.1186299999999996</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="13">
         <v>-34.913719999999998</v>
       </c>
       <c r="E12">
@@ -1457,15 +1458,15 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B13" t="s">
-        <v>123</v>
-      </c>
-      <c r="C13">
+        <v>121</v>
+      </c>
+      <c r="C13" s="13">
         <v>-8.1115499999999994</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="13">
         <v>-34.91234</v>
       </c>
       <c r="E13">
@@ -1477,15 +1478,15 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B14" t="s">
-        <v>123</v>
-      </c>
-      <c r="C14">
+        <v>121</v>
+      </c>
+      <c r="C14" s="13">
         <v>-8.1089400000000005</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="13">
         <v>-34.911799999999999</v>
       </c>
       <c r="E14">
@@ -1497,15 +1498,15 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B15" t="s">
-        <v>123</v>
-      </c>
-      <c r="C15">
+        <v>121</v>
+      </c>
+      <c r="C15" s="13">
         <v>-8.1061999999999994</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="13">
         <v>-34.911259999999999</v>
       </c>
       <c r="E15">
@@ -1517,15 +1518,15 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B16" t="s">
-        <v>119</v>
-      </c>
-      <c r="C16">
+        <v>117</v>
+      </c>
+      <c r="C16" s="13">
         <v>-8.0472400000000004</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="13">
         <v>-34.891530000000003</v>
       </c>
       <c r="E16">
@@ -1537,15 +1538,15 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B17" t="s">
-        <v>119</v>
-      </c>
-      <c r="C17">
+        <v>117</v>
+      </c>
+      <c r="C17" s="13">
         <v>-8.0501900000000006</v>
       </c>
-      <c r="D17">
+      <c r="D17" s="13">
         <v>-34.894350000000003</v>
       </c>
       <c r="E17">
@@ -1557,35 +1558,35 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B18" t="s">
-        <v>119</v>
-      </c>
-      <c r="C18">
+        <v>117</v>
+      </c>
+      <c r="C18" s="13">
         <v>-8.0502800000000008</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="13">
         <v>-34.893889999999999</v>
       </c>
       <c r="E18">
         <v>3</v>
       </c>
       <c r="F18">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B19" t="s">
-        <v>119</v>
-      </c>
-      <c r="C19">
+        <v>117</v>
+      </c>
+      <c r="C19" s="13">
         <v>-8.0542800000000003</v>
       </c>
-      <c r="D19">
+      <c r="D19" s="13">
         <v>-34.896850000000001</v>
       </c>
       <c r="E19">
@@ -1597,15 +1598,15 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B20" t="s">
-        <v>119</v>
-      </c>
-      <c r="C20">
+        <v>117</v>
+      </c>
+      <c r="C20" s="13">
         <v>-8.0571900000000003</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="13">
         <v>-34.898229999999998</v>
       </c>
       <c r="E20">
@@ -1617,15 +1618,15 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="C21">
+        <v>136</v>
+      </c>
+      <c r="C21" s="13">
         <v>-8.0796600000000005</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="13">
         <v>-34.93374</v>
       </c>
       <c r="E21">
@@ -1637,15 +1638,15 @@
     </row>
     <row r="22" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C22" s="7">
+        <v>122</v>
+      </c>
+      <c r="C22" s="13">
         <v>-8.1066699999999994</v>
       </c>
-      <c r="D22" s="7">
+      <c r="D22" s="13">
         <v>-34.927349999999997</v>
       </c>
       <c r="E22" s="7">
@@ -1657,15 +1658,15 @@
     </row>
     <row r="23" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="C23" s="7">
+        <v>122</v>
+      </c>
+      <c r="C23" s="13">
         <v>-8.1077700000000004</v>
       </c>
-      <c r="D23" s="7">
+      <c r="D23" s="13">
         <v>-34.927169999999997</v>
       </c>
       <c r="E23" s="7">
@@ -1677,15 +1678,15 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B24" t="s">
-        <v>127</v>
-      </c>
-      <c r="C24">
+        <v>125</v>
+      </c>
+      <c r="C24" s="13">
         <v>-8.0779700000000005</v>
       </c>
-      <c r="D24">
+      <c r="D24" s="13">
         <v>-34.89781</v>
       </c>
       <c r="E24">
@@ -1697,15 +1698,15 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="C25">
+        <v>133</v>
+      </c>
+      <c r="C25" s="13">
         <v>-8.0017399999999999</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="13">
         <v>-34.923749999999998</v>
       </c>
       <c r="E25">
@@ -1717,15 +1718,15 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="C26">
+        <v>132</v>
+      </c>
+      <c r="C26" s="13">
         <v>-8.0254999999999992</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="13">
         <v>-34.906619999999997</v>
       </c>
       <c r="E26">
@@ -1737,15 +1738,15 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B27" t="s">
-        <v>129</v>
-      </c>
-      <c r="C27">
+        <v>127</v>
+      </c>
+      <c r="C27" s="13">
         <v>-8.0549599999999995</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="13">
         <v>-34.895820000000001</v>
       </c>
       <c r="E27">
@@ -1757,15 +1758,15 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="C28">
+        <v>131</v>
+      </c>
+      <c r="C28" s="13">
         <v>-8.0661900000000006</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="13">
         <v>-34.889449999999997</v>
       </c>
       <c r="E28">
@@ -1777,15 +1778,15 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B29" t="s">
-        <v>122</v>
-      </c>
-      <c r="C29">
+        <v>120</v>
+      </c>
+      <c r="C29" s="13">
         <v>-8.0796600000000005</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="13">
         <v>-34.904530000000001</v>
       </c>
       <c r="E29">
@@ -1797,15 +1798,15 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" t="s">
         <v>128</v>
       </c>
-      <c r="B30" t="s">
-        <v>130</v>
-      </c>
-      <c r="C30">
+      <c r="C30" s="13">
         <v>-8.0782000000000007</v>
       </c>
-      <c r="D30">
+      <c r="D30" s="13">
         <v>-34.905520000000003</v>
       </c>
       <c r="E30">
@@ -1817,15 +1818,15 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="C31">
+        <v>138</v>
+      </c>
+      <c r="C31" s="13">
         <v>-8.1105800000000006</v>
       </c>
-      <c r="D31">
+      <c r="D31" s="13">
         <v>-34.937100000000001</v>
       </c>
       <c r="E31">
@@ -1837,15 +1838,15 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="C32">
+        <v>139</v>
+      </c>
+      <c r="C32" s="13">
         <v>-8.1229300000000002</v>
       </c>
-      <c r="D32">
+      <c r="D32" s="13">
         <v>-34.903959999999998</v>
       </c>
       <c r="E32">
@@ -1857,15 +1858,15 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B33" t="s">
-        <v>125</v>
-      </c>
-      <c r="C33">
+        <v>123</v>
+      </c>
+      <c r="C33" s="13">
         <v>-8.1418700000000008</v>
       </c>
-      <c r="D33">
+      <c r="D33" s="13">
         <v>-34.918700000000001</v>
       </c>
       <c r="E33">
@@ -1877,15 +1878,15 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B34" t="s">
-        <v>81</v>
-      </c>
-      <c r="C34" s="11">
+        <v>79</v>
+      </c>
+      <c r="C34" s="13">
         <v>-8.0629100000000005</v>
       </c>
-      <c r="D34" s="11">
+      <c r="D34" s="13">
         <v>-34.871960000000001</v>
       </c>
       <c r="E34">
@@ -1897,15 +1898,15 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B35" t="s">
-        <v>145</v>
-      </c>
-      <c r="C35" s="11">
+        <v>143</v>
+      </c>
+      <c r="C35" s="13">
         <v>-8.0658437972273997</v>
       </c>
-      <c r="D35" s="11">
+      <c r="D35" s="13">
         <v>-34.879644548383098</v>
       </c>
       <c r="E35">
@@ -1917,16 +1918,16 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B36" t="s">
-        <v>84</v>
-      </c>
-      <c r="C36">
-        <v>-8.0652100000000004</v>
-      </c>
-      <c r="D36">
-        <v>-34.876049999999999</v>
+        <v>82</v>
+      </c>
+      <c r="C36" s="13">
+        <v>-8.0596910799380197</v>
+      </c>
+      <c r="D36" s="13">
+        <v>-34.869988064354096</v>
       </c>
       <c r="E36">
         <v>42</v>
@@ -1936,16 +1937,16 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="12" t="s">
-        <v>147</v>
+      <c r="A37" s="11" t="s">
+        <v>145</v>
       </c>
       <c r="B37" t="s">
-        <v>59</v>
-      </c>
-      <c r="C37" s="11">
+        <v>57</v>
+      </c>
+      <c r="C37" s="13">
         <v>-8.0561880640993202</v>
       </c>
-      <c r="D37" s="11">
+      <c r="D37" s="13">
         <v>-34.877104862147597</v>
       </c>
       <c r="E37">
@@ -1957,15 +1958,15 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B38" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" s="11">
+        <v>23</v>
+      </c>
+      <c r="C38" s="13">
         <v>-8.031604626120016</v>
       </c>
-      <c r="D38" s="11">
+      <c r="D38" s="13">
         <v>-34.924639637975957</v>
       </c>
       <c r="E38">
@@ -1977,15 +1978,15 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
-      </c>
-      <c r="C39" s="8">
+        <v>77</v>
+      </c>
+      <c r="C39" s="13">
         <v>-8.0631233071071193</v>
       </c>
-      <c r="D39" s="9">
+      <c r="D39" s="13">
         <v>-34.8710022666098</v>
       </c>
       <c r="E39">
@@ -1997,15 +1998,15 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B40" t="s">
-        <v>91</v>
-      </c>
-      <c r="C40">
+        <v>89</v>
+      </c>
+      <c r="C40" s="13">
         <v>-8.0632113000000007</v>
       </c>
-      <c r="D40">
+      <c r="D40" s="13">
         <v>-34.891190299999998</v>
       </c>
       <c r="E40">
@@ -2017,15 +2018,15 @@
     </row>
     <row r="41" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C41" s="4">
+        <v>18</v>
+      </c>
+      <c r="C41" s="13">
         <v>-8.0373614419372608</v>
       </c>
-      <c r="D41" s="4">
+      <c r="D41" s="13">
         <v>-34.892167160062002</v>
       </c>
       <c r="E41" s="4">
@@ -2037,15 +2038,15 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B42" t="s">
-        <v>35</v>
-      </c>
-      <c r="C42">
+        <v>33</v>
+      </c>
+      <c r="C42" s="13">
         <v>-8.0523349999999994</v>
       </c>
-      <c r="D42">
+      <c r="D42" s="13">
         <v>-34.908380000000001</v>
       </c>
       <c r="E42">
@@ -2057,15 +2058,15 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B43" t="s">
-        <v>111</v>
-      </c>
-      <c r="C43">
+        <v>109</v>
+      </c>
+      <c r="C43" s="13">
         <v>-8.0443764000000009</v>
       </c>
-      <c r="D43">
+      <c r="D43" s="13">
         <v>-34.910375999999999</v>
       </c>
       <c r="E43">
@@ -2077,15 +2078,15 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B44" t="s">
-        <v>93</v>
-      </c>
-      <c r="C44">
+        <v>91</v>
+      </c>
+      <c r="C44" s="13">
         <v>-8.0710313649999996</v>
       </c>
-      <c r="D44">
+      <c r="D44" s="13">
         <v>-34.877230730000001</v>
       </c>
       <c r="E44">
@@ -2097,15 +2098,15 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B45" t="s">
-        <v>130</v>
-      </c>
-      <c r="C45">
+        <v>128</v>
+      </c>
+      <c r="C45" s="13">
         <v>-8.0774484770977697</v>
       </c>
-      <c r="D45">
+      <c r="D45" s="13">
         <v>-34.906173347262097</v>
       </c>
       <c r="E45">
@@ -2117,15 +2118,15 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B46" t="s">
-        <v>110</v>
-      </c>
-      <c r="C46">
+        <v>108</v>
+      </c>
+      <c r="C46" s="13">
         <v>-8.019325791</v>
       </c>
-      <c r="D46">
+      <c r="D46" s="13">
         <v>-34.893893419999998</v>
       </c>
       <c r="E46">
@@ -2137,15 +2138,15 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B47" t="s">
-        <v>109</v>
-      </c>
-      <c r="C47">
+        <v>107</v>
+      </c>
+      <c r="C47" s="13">
         <v>-8.0026340841323993</v>
       </c>
-      <c r="D47">
+      <c r="D47" s="13">
         <v>-34.897381311996803</v>
       </c>
       <c r="E47">
@@ -2157,15 +2158,15 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B48" t="s">
-        <v>86</v>
-      </c>
-      <c r="C48">
+        <v>84</v>
+      </c>
+      <c r="C48" s="13">
         <v>-8.0262613999999992</v>
       </c>
-      <c r="D48">
+      <c r="D48" s="13">
         <v>-34.920241699999998</v>
       </c>
       <c r="E48">
@@ -2177,15 +2178,15 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B49" t="s">
-        <v>108</v>
-      </c>
-      <c r="C49">
+        <v>106</v>
+      </c>
+      <c r="C49" s="13">
         <v>-8.0466867719999993</v>
       </c>
-      <c r="D49">
+      <c r="D49" s="13">
         <v>-34.876619990000002</v>
       </c>
       <c r="E49">
@@ -2197,15 +2198,15 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B50" t="s">
-        <v>68</v>
-      </c>
-      <c r="C50" s="11">
+        <v>66</v>
+      </c>
+      <c r="C50" s="13">
         <v>-8.0683118247106602</v>
       </c>
-      <c r="D50" s="11">
+      <c r="D50" s="13">
         <v>-34.877617084802701</v>
       </c>
       <c r="E50">
@@ -2217,15 +2218,15 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B51" t="s">
-        <v>3</v>
-      </c>
-      <c r="C51">
+        <v>1</v>
+      </c>
+      <c r="C51" s="13">
         <v>-8.0518440560000002</v>
       </c>
-      <c r="D51">
+      <c r="D51" s="13">
         <v>-34.921453929999998</v>
       </c>
       <c r="E51">
@@ -2237,15 +2238,15 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B52" t="s">
-        <v>112</v>
-      </c>
-      <c r="C52">
+        <v>110</v>
+      </c>
+      <c r="C52" s="13">
         <v>-8.0871689789999994</v>
       </c>
-      <c r="D52">
+      <c r="D52" s="13">
         <v>-34.882869679999999</v>
       </c>
       <c r="E52">
@@ -2257,15 +2258,15 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B53" t="s">
-        <v>42</v>
-      </c>
-      <c r="C53" s="8">
+        <v>40</v>
+      </c>
+      <c r="C53" s="13">
         <v>-8.0918133099417098</v>
       </c>
-      <c r="D53" s="9">
+      <c r="D53" s="13">
         <v>-34.881938263926898</v>
       </c>
       <c r="E53">
@@ -2277,15 +2278,15 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B54" t="s">
-        <v>107</v>
-      </c>
-      <c r="C54" s="11">
+        <v>105</v>
+      </c>
+      <c r="C54" s="13">
         <v>-8.1169846559999996</v>
       </c>
-      <c r="D54" s="11">
+      <c r="D54" s="13">
         <v>-34.912922829999999</v>
       </c>
       <c r="E54">
@@ -2297,15 +2298,15 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B55" t="s">
-        <v>83</v>
-      </c>
-      <c r="C55" s="8">
+        <v>81</v>
+      </c>
+      <c r="C55" s="13">
         <v>-8.0647000000000002</v>
       </c>
-      <c r="D55" s="9">
+      <c r="D55" s="13">
         <v>-34.87379</v>
       </c>
       <c r="E55">
@@ -2317,15 +2318,15 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B56" t="s">
-        <v>153</v>
-      </c>
-      <c r="C56">
+        <v>151</v>
+      </c>
+      <c r="C56" s="13">
         <v>-8.0933499999999992</v>
       </c>
-      <c r="D56">
+      <c r="D56" s="13">
         <v>-34.892569999999999</v>
       </c>
       <c r="E56">
@@ -2337,15 +2338,15 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B57" t="s">
-        <v>16</v>
-      </c>
-      <c r="C57">
+        <v>14</v>
+      </c>
+      <c r="C57" s="13">
         <v>-8.1032904511294284</v>
       </c>
-      <c r="D57">
+      <c r="D57" s="13">
         <v>-34.938219328046898</v>
       </c>
       <c r="E57">
@@ -2357,15 +2358,15 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B58" t="s">
-        <v>13</v>
-      </c>
-      <c r="C58" s="11">
+        <v>11</v>
+      </c>
+      <c r="C58" s="13">
         <v>-8.0571900000000003</v>
       </c>
-      <c r="D58" s="11">
+      <c r="D58" s="13">
         <v>-34.943100000000001</v>
       </c>
       <c r="E58">
@@ -2377,15 +2378,15 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B59" t="s">
-        <v>30</v>
-      </c>
-      <c r="C59" s="8">
+        <v>28</v>
+      </c>
+      <c r="C59" s="13">
         <v>-8.03037578</v>
       </c>
-      <c r="D59" s="9">
+      <c r="D59" s="13">
         <v>-34.91302219</v>
       </c>
       <c r="E59">
@@ -2397,15 +2398,15 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B60" t="s">
-        <v>19</v>
-      </c>
-      <c r="C60" s="11">
+        <v>17</v>
+      </c>
+      <c r="C60" s="13">
         <v>-8.0152591867061407</v>
       </c>
-      <c r="D60" s="11">
+      <c r="D60" s="13">
         <v>-34.932259581601897</v>
       </c>
       <c r="E60">
@@ -2417,15 +2418,15 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B61" t="s">
-        <v>46</v>
-      </c>
-      <c r="C61" s="11">
+        <v>44</v>
+      </c>
+      <c r="C61" s="13">
         <v>-8.0455253553702306</v>
       </c>
-      <c r="D61" s="11">
+      <c r="D61" s="13">
         <v>-34.902801244642703</v>
       </c>
       <c r="E61">
@@ -2437,15 +2438,15 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B62" t="s">
-        <v>17</v>
-      </c>
-      <c r="C62" s="11">
+        <v>15</v>
+      </c>
+      <c r="C62" s="13">
         <v>-8.0388800000000007</v>
       </c>
-      <c r="D62" s="11">
+      <c r="D62" s="13">
         <v>-34.927500000000002</v>
       </c>
       <c r="E62">
@@ -2457,15 +2458,15 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B63" t="s">
-        <v>85</v>
-      </c>
-      <c r="C63" s="11">
+        <v>83</v>
+      </c>
+      <c r="C63" s="13">
         <v>-8.0133542866917402</v>
       </c>
-      <c r="D63" s="11">
+      <c r="D63" s="13">
         <v>-34.944212082769504</v>
       </c>
       <c r="E63">
@@ -2477,15 +2478,15 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>156</v>
-      </c>
-      <c r="C64">
+        <v>154</v>
+      </c>
+      <c r="C64" s="13">
         <v>-8.0757700000000003</v>
       </c>
-      <c r="D64">
+      <c r="D64" s="13">
         <v>-34.889209999999999</v>
       </c>
       <c r="E64">
@@ -2497,15 +2498,15 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B65" t="s">
-        <v>158</v>
-      </c>
-      <c r="C65">
+        <v>156</v>
+      </c>
+      <c r="C65" s="13">
         <v>-8.0682399999999994</v>
       </c>
-      <c r="D65">
+      <c r="D65" s="13">
         <v>-34.893129999999999</v>
       </c>
       <c r="E65">
@@ -2517,15 +2518,15 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B66" t="s">
-        <v>63</v>
-      </c>
-      <c r="C66">
+        <v>61</v>
+      </c>
+      <c r="C66" s="13">
         <v>-8.0568018479999992</v>
       </c>
-      <c r="D66">
+      <c r="D66" s="13">
         <v>-34.881540399999999</v>
       </c>
       <c r="E66">
@@ -2537,15 +2538,15 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B67" t="s">
-        <v>12</v>
-      </c>
-      <c r="C67">
+        <v>10</v>
+      </c>
+      <c r="C67" s="13">
         <v>-8.0670076769999994</v>
       </c>
-      <c r="D67">
+      <c r="D67" s="13">
         <v>-34.878943710000001</v>
       </c>
       <c r="E67">
@@ -2557,15 +2558,15 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B68" t="s">
-        <v>72</v>
-      </c>
-      <c r="C68" s="11">
+        <v>70</v>
+      </c>
+      <c r="C68" s="13">
         <v>-8.0671258986764194</v>
       </c>
-      <c r="D68" s="11">
+      <c r="D68" s="13">
         <v>-34.878057535739302</v>
       </c>
       <c r="E68">
@@ -2577,15 +2578,15 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B69" t="s">
-        <v>110</v>
-      </c>
-      <c r="C69" s="8">
+        <v>108</v>
+      </c>
+      <c r="C69" s="13">
         <v>-8.0030395589999994</v>
       </c>
-      <c r="D69" s="9">
+      <c r="D69" s="13">
         <v>-34.897848570000001</v>
       </c>
       <c r="E69">
@@ -2597,15 +2598,15 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B70" t="s">
-        <v>42</v>
-      </c>
-      <c r="C70" s="8">
+        <v>40</v>
+      </c>
+      <c r="C70" s="13">
         <v>-8.1059000000000001</v>
       </c>
-      <c r="D70" s="9">
+      <c r="D70" s="13">
         <v>-34.887700000000002</v>
       </c>
       <c r="E70">
@@ -2617,16 +2618,16 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B71" t="s">
-        <v>42</v>
-      </c>
-      <c r="C71" s="8">
-        <v>-8.10501</v>
-      </c>
-      <c r="D71" s="9">
-        <v>-34.887</v>
+        <v>40</v>
+      </c>
+      <c r="C71" s="19">
+        <v>-8108306</v>
+      </c>
+      <c r="D71" s="19">
+        <v>-34888487</v>
       </c>
       <c r="E71">
         <v>89</v>
@@ -2637,10 +2638,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B72" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C72" s="8">
         <v>-8.1020699999999994</v>
@@ -2657,10 +2658,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B73" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C73">
         <v>-8.0354030999999999</v>
@@ -2676,16 +2677,16 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>36</v>
+      <c r="A74" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="B74" t="s">
-        <v>37</v>
-      </c>
-      <c r="C74" s="11">
+        <v>35</v>
+      </c>
+      <c r="C74" s="20">
         <v>-8.0029137349999999</v>
       </c>
-      <c r="D74" s="11">
+      <c r="D74" s="20">
         <v>-34.907381350000001</v>
       </c>
       <c r="E74">
@@ -2696,11 +2697,11 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>6</v>
+      <c r="A75" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="B75" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C75">
         <v>-8.0917032715727704</v>
@@ -2717,10 +2718,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B76" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C76" s="8">
         <v>-8.054316900326878</v>
@@ -2737,15 +2738,15 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B77" t="s">
-        <v>40</v>
-      </c>
-      <c r="C77" s="11">
+        <v>38</v>
+      </c>
+      <c r="C77" s="20">
         <v>-8.0506795404506857</v>
       </c>
-      <c r="D77" s="11">
+      <c r="D77" s="20">
         <v>-34.907087309499254</v>
       </c>
       <c r="E77">
@@ -2757,10 +2758,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B78" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C78">
         <v>-8.1057745109999999</v>
@@ -2777,15 +2778,15 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B79" t="s">
-        <v>10</v>
-      </c>
-      <c r="C79" s="11">
+        <v>8</v>
+      </c>
+      <c r="C79" s="20">
         <v>-8.1209634325435704</v>
       </c>
-      <c r="D79" s="11">
+      <c r="D79" s="20">
         <v>-34.945930972484199</v>
       </c>
       <c r="E79">
@@ -2797,10 +2798,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B80" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C80" s="8">
         <v>-8.0335093116039573</v>
@@ -2817,10 +2818,10 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B81" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C81">
         <v>-8.057972572465788</v>
@@ -2837,10 +2838,10 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B82" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C82">
         <v>-8.0707956549572497</v>
@@ -2857,15 +2858,15 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B83" t="s">
-        <v>70</v>
-      </c>
-      <c r="C83" s="11">
+        <v>68</v>
+      </c>
+      <c r="C83" s="20">
         <v>-8.0609670624366405</v>
       </c>
-      <c r="D83" s="11">
+      <c r="D83" s="20">
         <v>-34.877245681326698</v>
       </c>
       <c r="E83">
@@ -2877,10 +2878,10 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B84" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C84" s="8">
         <v>-8.0491004724083695</v>
@@ -2897,10 +2898,10 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B85" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C85" s="8">
         <v>-8.1183840561139409</v>
@@ -2917,16 +2918,16 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B86" t="s">
-        <v>48</v>
-      </c>
-      <c r="C86">
-        <v>-8.1318453757380595</v>
-      </c>
-      <c r="D86">
-        <v>-34.899977714417403</v>
+        <v>46</v>
+      </c>
+      <c r="C86" s="21">
+        <v>-8132158</v>
+      </c>
+      <c r="D86" s="1">
+        <v>-34900280</v>
       </c>
       <c r="E86">
         <v>109</v>
@@ -2937,15 +2938,15 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B87" t="s">
-        <v>25</v>
-      </c>
-      <c r="C87" s="11">
+        <v>23</v>
+      </c>
+      <c r="C87" s="20">
         <v>-8.0347728739999997</v>
       </c>
-      <c r="D87" s="11">
+      <c r="D87" s="20">
         <v>-34.919505219999998</v>
       </c>
       <c r="E87">
@@ -2957,15 +2958,15 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B88" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" s="11">
+        <v>3</v>
+      </c>
+      <c r="C88" s="20">
         <v>-8.0610589800000003</v>
       </c>
-      <c r="D88" s="11">
+      <c r="D88" s="20">
         <v>-34.871273469999998</v>
       </c>
       <c r="E88">
@@ -2977,15 +2978,15 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B89" t="s">
-        <v>19</v>
-      </c>
-      <c r="C89" s="11">
+        <v>17</v>
+      </c>
+      <c r="C89" s="20">
         <v>-8.0234482595867505</v>
       </c>
-      <c r="D89" s="11">
+      <c r="D89" s="20">
         <v>-34.914670590409798</v>
       </c>
       <c r="E89">
@@ -2997,15 +2998,15 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B90" t="s">
-        <v>68</v>
-      </c>
-      <c r="C90" s="11">
+        <v>66</v>
+      </c>
+      <c r="C90" s="20">
         <v>-8.0682260813088291</v>
       </c>
-      <c r="D90" s="11">
+      <c r="D90" s="20">
         <v>-34.878422989818198</v>
       </c>
       <c r="E90">
@@ -3017,19 +3018,19 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="B91" t="s">
-        <v>68</v>
-      </c>
-      <c r="C91">
-        <v>-8.0686411420000006</v>
-      </c>
-      <c r="D91">
-        <v>-34.880234899999998</v>
+        <v>36</v>
+      </c>
+      <c r="C91" s="20">
+        <v>-8.0410776736114098</v>
+      </c>
+      <c r="D91" s="20">
+        <v>-34.904317758007501</v>
       </c>
       <c r="E91">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="F91">
         <v>3</v>
@@ -3037,19 +3038,19 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>41</v>
+        <v>221</v>
       </c>
       <c r="B92" t="s">
-        <v>38</v>
-      </c>
-      <c r="C92" s="11">
-        <v>-8.0410776736114098</v>
-      </c>
-      <c r="D92" s="11">
-        <v>-34.904317758007501</v>
+        <v>222</v>
+      </c>
+      <c r="C92">
+        <v>-8.0565599999999993</v>
+      </c>
+      <c r="D92">
+        <v>-34.9</v>
       </c>
       <c r="E92">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="F92">
         <v>3</v>
@@ -3057,19 +3058,19 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>223</v>
+        <v>95</v>
       </c>
       <c r="B93" t="s">
-        <v>224</v>
-      </c>
-      <c r="C93">
-        <v>-8.0565599999999993</v>
-      </c>
-      <c r="D93">
-        <v>-34.9</v>
+        <v>112</v>
+      </c>
+      <c r="C93" s="20">
+        <v>-8.0267300000000006</v>
+      </c>
+      <c r="D93" s="20">
+        <v>-34.918700000000001</v>
       </c>
       <c r="E93">
-        <v>114</v>
+        <v>101</v>
       </c>
       <c r="F93">
         <v>3</v>
@@ -3077,19 +3078,19 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="B94" t="s">
-        <v>114</v>
-      </c>
-      <c r="C94" s="11">
-        <v>-8.0267300000000006</v>
-      </c>
-      <c r="D94" s="11">
-        <v>-34.918700000000001</v>
+        <v>31</v>
+      </c>
+      <c r="C94">
+        <v>-8.0945099999999996</v>
+      </c>
+      <c r="D94">
+        <v>-34.913899999999998</v>
       </c>
       <c r="E94">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="F94">
         <v>3</v>
@@ -3097,19 +3098,19 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>32</v>
+        <v>96</v>
       </c>
       <c r="B95" t="s">
-        <v>33</v>
-      </c>
-      <c r="C95">
-        <v>-8.0945099999999996</v>
-      </c>
-      <c r="D95">
-        <v>-34.913899999999998</v>
+        <v>111</v>
+      </c>
+      <c r="C95" s="20">
+        <v>-8.0209019323429107</v>
+      </c>
+      <c r="D95" s="20">
+        <v>-34.917366133765498</v>
       </c>
       <c r="E95">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F95">
         <v>3</v>
@@ -3117,19 +3118,19 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>98</v>
+        <v>53</v>
       </c>
       <c r="B96" t="s">
-        <v>113</v>
-      </c>
-      <c r="C96" s="11">
-        <v>-8.0209019323429107</v>
-      </c>
-      <c r="D96" s="11">
-        <v>-34.917366133765498</v>
+        <v>54</v>
+      </c>
+      <c r="C96" s="20">
+        <v>-8.0622754000000008</v>
+      </c>
+      <c r="D96" s="20">
+        <v>-34.885648099999997</v>
       </c>
       <c r="E96">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="F96">
         <v>3</v>
@@ -3137,19 +3138,19 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="B97" t="s">
-        <v>56</v>
-      </c>
-      <c r="C97" s="11">
-        <v>-8.0622754000000008</v>
-      </c>
-      <c r="D97" s="11">
-        <v>-34.885648099999997</v>
+        <v>51</v>
+      </c>
+      <c r="C97" s="20">
+        <v>-8.0725033140000004</v>
+      </c>
+      <c r="D97" s="20">
+        <v>-34.886144160000001</v>
       </c>
       <c r="E97">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="F97">
         <v>3</v>
@@ -3157,19 +3158,19 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>52</v>
+        <v>24</v>
       </c>
       <c r="B98" t="s">
-        <v>53</v>
-      </c>
-      <c r="C98" s="11">
-        <v>-8.0725033140000004</v>
-      </c>
-      <c r="D98" s="11">
-        <v>-34.886144160000001</v>
+        <v>23</v>
+      </c>
+      <c r="C98" s="20">
+        <v>-8.0313872200619407</v>
+      </c>
+      <c r="D98" s="20">
+        <v>-34.924635268843282</v>
       </c>
       <c r="E98">
-        <v>93</v>
+        <v>120</v>
       </c>
       <c r="F98">
         <v>3</v>
@@ -3177,39 +3178,39 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>26</v>
+        <v>158</v>
       </c>
       <c r="B99" t="s">
-        <v>25</v>
-      </c>
-      <c r="C99" s="11">
-        <v>-8.0313872200619407</v>
-      </c>
-      <c r="D99" s="11">
-        <v>-34.924635268843282</v>
+        <v>80</v>
+      </c>
+      <c r="C99" s="20">
+        <v>-8.0646199999999997</v>
+      </c>
+      <c r="D99" s="20">
+        <v>-34.872889999999998</v>
       </c>
       <c r="E99">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F99">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B100" t="s">
-        <v>82</v>
-      </c>
-      <c r="C100" s="11">
-        <v>-8.0646199999999997</v>
-      </c>
-      <c r="D100" s="11">
-        <v>-34.872889999999998</v>
+        <v>3</v>
+      </c>
+      <c r="C100" s="8">
+        <v>-8.0619899999999998</v>
+      </c>
+      <c r="D100" s="9">
+        <v>-34.871519999999997</v>
       </c>
       <c r="E100">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="F100">
         <v>1</v>
@@ -3217,79 +3218,79 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
+        <v>160</v>
+      </c>
+      <c r="B101" t="s">
         <v>161</v>
       </c>
-      <c r="B101" t="s">
-        <v>5</v>
-      </c>
-      <c r="C101" s="8">
-        <v>-8.0619899999999998</v>
-      </c>
-      <c r="D101" s="9">
-        <v>-34.871519999999997</v>
+      <c r="C101">
+        <v>-8.0191721076781093</v>
+      </c>
+      <c r="D101">
+        <v>-34.915538393356499</v>
       </c>
       <c r="E101">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F101">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>162</v>
+        <v>93</v>
       </c>
       <c r="B102" t="s">
-        <v>163</v>
-      </c>
-      <c r="C102">
-        <v>-8.0191721076781093</v>
-      </c>
-      <c r="D102">
-        <v>-34.915538393356499</v>
+        <v>28</v>
+      </c>
+      <c r="C102" s="22">
+        <v>-8.0305944</v>
+      </c>
+      <c r="D102" s="23">
+        <v>-34.915496099999999</v>
       </c>
       <c r="E102">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F102">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="B103" t="s">
-        <v>30</v>
-      </c>
-      <c r="C103" s="13">
-        <v>-8.0305944</v>
-      </c>
-      <c r="D103" s="14">
-        <v>-34.915496099999999</v>
+        <v>75</v>
+      </c>
+      <c r="C103" s="20">
+        <v>-8.0613100000000006</v>
+      </c>
+      <c r="D103" s="20">
+        <v>-34.872509999999998</v>
       </c>
       <c r="E103">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F103">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>76</v>
+        <v>58</v>
       </c>
       <c r="B104" t="s">
-        <v>77</v>
-      </c>
-      <c r="C104" s="11">
-        <v>-8.0613100000000006</v>
-      </c>
-      <c r="D104" s="11">
-        <v>-34.872509999999998</v>
+        <v>59</v>
+      </c>
+      <c r="C104" s="21">
+        <v>-8090593</v>
+      </c>
+      <c r="D104">
+        <v>-34.884158999999997</v>
       </c>
       <c r="E104">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F104">
         <v>1</v>
@@ -3297,19 +3298,19 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>60</v>
+        <v>67</v>
       </c>
       <c r="B105" t="s">
-        <v>61</v>
-      </c>
-      <c r="C105">
-        <v>-8.0896899999999992</v>
-      </c>
-      <c r="D105">
-        <v>-34.882640000000002</v>
+        <v>68</v>
+      </c>
+      <c r="C105" s="20">
+        <v>-8.0605799999999999</v>
+      </c>
+      <c r="D105" s="20">
+        <v>-34.878079999999997</v>
       </c>
       <c r="E105">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F105">
         <v>1</v>
@@ -3317,19 +3318,19 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B106" t="s">
-        <v>70</v>
-      </c>
-      <c r="C106" s="11">
-        <v>-8.0605799999999999</v>
-      </c>
-      <c r="D106" s="11">
-        <v>-34.878079999999997</v>
+        <v>56</v>
+      </c>
+      <c r="C106">
+        <v>-8.0618400000000001</v>
+      </c>
+      <c r="D106">
+        <v>-34.884700000000002</v>
       </c>
       <c r="E106">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F106">
         <v>1</v>
@@ -3337,19 +3338,19 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="B107" t="s">
-        <v>58</v>
-      </c>
-      <c r="C107">
-        <v>-8.0618400000000001</v>
-      </c>
-      <c r="D107">
-        <v>-34.884700000000002</v>
+        <v>73</v>
+      </c>
+      <c r="C107" s="8">
+        <v>-8.0610499999999998</v>
+      </c>
+      <c r="D107" s="9">
+        <v>-34.872990000000001</v>
       </c>
       <c r="E107">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="F107">
         <v>1</v>
@@ -3357,39 +3358,39 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>74</v>
-      </c>
-      <c r="B108" t="s">
-        <v>75</v>
-      </c>
-      <c r="C108" s="8">
-        <v>-8.0610499999999998</v>
-      </c>
-      <c r="D108" s="9">
-        <v>-34.872990000000001</v>
+        <v>162</v>
+      </c>
+      <c r="B108" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="C108" s="12">
+        <v>-8.0506770000000003</v>
+      </c>
+      <c r="D108" s="12">
+        <v>-34.872959999999999</v>
       </c>
       <c r="E108">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F108">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>164</v>
-      </c>
-      <c r="B109" s="15" t="s">
-        <v>164</v>
-      </c>
-      <c r="C109" s="15">
-        <v>-8.0506770000000003</v>
-      </c>
-      <c r="D109" s="15">
-        <v>-34.872959999999999</v>
+        <v>163</v>
+      </c>
+      <c r="B109" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="C109" s="12">
+        <v>-8.06386</v>
+      </c>
+      <c r="D109" s="12">
+        <v>-34.875390000000003</v>
       </c>
       <c r="E109">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="F109">
         <v>2</v>
@@ -3397,19 +3398,19 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>165</v>
-      </c>
-      <c r="B110" s="15" t="s">
-        <v>165</v>
-      </c>
-      <c r="C110" s="15">
-        <v>-8.06386</v>
-      </c>
-      <c r="D110" s="15">
-        <v>-34.875390000000003</v>
+        <v>164</v>
+      </c>
+      <c r="B110" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="C110" s="12">
+        <v>-8.0619700000000005</v>
+      </c>
+      <c r="D110" s="12">
+        <v>-34.875079999999997</v>
       </c>
       <c r="E110">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F110">
         <v>2</v>
@@ -3417,19 +3418,19 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>166</v>
-      </c>
-      <c r="B111" s="15" t="s">
-        <v>166</v>
-      </c>
-      <c r="C111" s="15">
-        <v>-8.0619700000000005</v>
-      </c>
-      <c r="D111" s="15">
-        <v>-34.875079999999997</v>
+        <v>165</v>
+      </c>
+      <c r="B111" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="C111" s="12">
+        <v>-8.0671199999999992</v>
+      </c>
+      <c r="D111" s="12">
+        <v>-34.873989999999999</v>
       </c>
       <c r="E111">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="F111">
         <v>2</v>
@@ -3437,19 +3438,19 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>167</v>
-      </c>
-      <c r="B112" s="15" t="s">
-        <v>167</v>
-      </c>
-      <c r="C112" s="15">
-        <v>-8.0671199999999992</v>
-      </c>
-      <c r="D112" s="15">
-        <v>-34.873989999999999</v>
+        <v>166</v>
+      </c>
+      <c r="B112" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="C112" s="12">
+        <v>-8.05992</v>
+      </c>
+      <c r="D112" s="12">
+        <v>-34.879330000000003</v>
       </c>
       <c r="E112">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="F112">
         <v>2</v>
@@ -3457,19 +3458,19 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>168</v>
-      </c>
-      <c r="B113" s="15" t="s">
-        <v>168</v>
-      </c>
-      <c r="C113" s="15">
-        <v>-8.05992</v>
-      </c>
-      <c r="D113" s="15">
-        <v>-34.879330000000003</v>
+        <v>167</v>
+      </c>
+      <c r="B113" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="C113" s="12">
+        <v>-8.0623199999999997</v>
+      </c>
+      <c r="D113" s="12">
+        <v>-34.881039999999999</v>
       </c>
       <c r="E113">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="F113">
         <v>2</v>
@@ -3477,19 +3478,19 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>169</v>
-      </c>
-      <c r="B114" s="15" t="s">
-        <v>169</v>
-      </c>
-      <c r="C114" s="15">
-        <v>-8.0623199999999997</v>
-      </c>
-      <c r="D114" s="15">
-        <v>-34.881039999999999</v>
+        <v>168</v>
+      </c>
+      <c r="B114" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="C114" s="12">
+        <v>-8.0659799999999997</v>
+      </c>
+      <c r="D114" s="12">
+        <v>-34.884689999999999</v>
       </c>
       <c r="E114">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="F114">
         <v>2</v>
@@ -3497,19 +3498,19 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>170</v>
-      </c>
-      <c r="B115" s="15" t="s">
-        <v>170</v>
-      </c>
-      <c r="C115" s="15">
-        <v>-8.0659799999999997</v>
-      </c>
-      <c r="D115" s="15">
-        <v>-34.884689999999999</v>
+        <v>169</v>
+      </c>
+      <c r="B115" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="C115" s="12">
+        <v>-8.045477</v>
+      </c>
+      <c r="D115" s="12">
+        <v>-8.045477</v>
       </c>
       <c r="E115">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="F115">
         <v>2</v>
@@ -3517,19 +3518,19 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>171</v>
-      </c>
-      <c r="B116" s="15" t="s">
-        <v>171</v>
-      </c>
-      <c r="C116" s="15">
-        <v>-8.045477</v>
-      </c>
-      <c r="D116" s="15">
-        <v>-8.045477</v>
+        <v>170</v>
+      </c>
+      <c r="B116" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C116" s="12">
+        <v>-8.0827240000000007</v>
+      </c>
+      <c r="D116" s="12">
+        <v>-34.890836999999998</v>
       </c>
       <c r="E116">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="F116">
         <v>2</v>
@@ -3537,19 +3538,19 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>172</v>
-      </c>
-      <c r="B117" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="C117" s="15">
-        <v>-8.0827240000000007</v>
-      </c>
-      <c r="D117" s="15">
-        <v>-34.890836999999998</v>
+        <v>170</v>
+      </c>
+      <c r="B117" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C117" s="12">
+        <v>-8.0822699999999994</v>
+      </c>
+      <c r="D117" s="12">
+        <v>-34.889646999999997</v>
       </c>
       <c r="E117">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F117">
         <v>2</v>
@@ -3557,39 +3558,39 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>172</v>
-      </c>
-      <c r="B118" s="15" t="s">
-        <v>176</v>
-      </c>
-      <c r="C118" s="15">
-        <v>-8.0822699999999994</v>
-      </c>
-      <c r="D118" s="15">
-        <v>-34.889646999999997</v>
+        <v>171</v>
+      </c>
+      <c r="B118" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="C118" s="12">
+        <v>-8.0577939999999995</v>
+      </c>
+      <c r="D118" s="12">
+        <v>-34.909590999999999</v>
       </c>
       <c r="E118">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="F118">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>173</v>
-      </c>
-      <c r="B119" s="15" t="s">
-        <v>173</v>
-      </c>
-      <c r="C119" s="15">
-        <v>-8.0577939999999995</v>
-      </c>
-      <c r="D119" s="15">
-        <v>-34.909590999999999</v>
+        <v>118</v>
+      </c>
+      <c r="B119" s="12" t="s">
+        <v>118</v>
+      </c>
+      <c r="C119" s="12">
+        <v>-8.0615539999999992</v>
+      </c>
+      <c r="D119" s="12">
+        <v>-34.901347999999999</v>
       </c>
       <c r="E119">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="F119">
         <v>1</v>
@@ -3597,19 +3598,19 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>120</v>
-      </c>
-      <c r="B120" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="C120" s="15">
-        <v>-8.0615539999999992</v>
-      </c>
-      <c r="D120" s="15">
-        <v>-34.901347999999999</v>
+        <v>172</v>
+      </c>
+      <c r="B120" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="C120" s="12">
+        <v>-8.0865039999999997</v>
+      </c>
+      <c r="D120" s="12">
+        <v>-34.888176000000001</v>
       </c>
       <c r="E120">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="F120">
         <v>1</v>
@@ -3617,19 +3618,19 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>174</v>
-      </c>
-      <c r="B121" s="15" t="s">
-        <v>174</v>
-      </c>
-      <c r="C121" s="15">
-        <v>-8.0865039999999997</v>
-      </c>
-      <c r="D121" s="15">
-        <v>-34.888176000000001</v>
+        <v>173</v>
+      </c>
+      <c r="B121" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="C121" s="12">
+        <v>-8.1233310000000003</v>
+      </c>
+      <c r="D121" s="12">
+        <v>-34.909514999999999</v>
       </c>
       <c r="E121">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="F121">
         <v>1</v>
@@ -3637,19 +3638,19 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>175</v>
-      </c>
-      <c r="B122" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="C122" s="15">
-        <v>-8.1233310000000003</v>
-      </c>
-      <c r="D122" s="15">
-        <v>-34.909514999999999</v>
+        <v>173</v>
+      </c>
+      <c r="B122" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="C122" s="12">
+        <v>-8.1232679999999995</v>
+      </c>
+      <c r="D122" s="12">
+        <v>-34.909429000000003</v>
       </c>
       <c r="E122">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="F122">
         <v>1</v>
@@ -3659,258 +3660,336 @@
       <c r="A123" t="s">
         <v>175</v>
       </c>
-      <c r="B123" s="15" t="s">
+      <c r="B123" s="12" t="s">
         <v>175</v>
       </c>
-      <c r="C123" s="15">
-        <v>-8.1232679999999995</v>
-      </c>
-      <c r="D123" s="15">
-        <v>-34.909429000000003</v>
+      <c r="C123" s="14">
+        <v>-8.1048700733912096</v>
+      </c>
+      <c r="D123" s="24">
+        <v>-34.891163918022997</v>
       </c>
       <c r="E123">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="F123">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A124" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A124" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="B124" s="18" t="s">
+        <v>223</v>
+      </c>
+      <c r="C124" s="25">
+        <v>-8.0635997672068793</v>
+      </c>
+      <c r="D124" s="25">
+        <v>-34.881890011734797</v>
+      </c>
+      <c r="E124">
+        <v>146</v>
+      </c>
+      <c r="F124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="B125" s="18" t="s">
+        <v>224</v>
+      </c>
+      <c r="C125" s="26">
+        <v>-8.0297949481864208</v>
+      </c>
+      <c r="D125" s="26">
+        <v>-34.929545690228501</v>
+      </c>
+      <c r="E125">
+        <v>147</v>
+      </c>
+      <c r="F125">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A126" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="B124" s="15" t="s">
-        <v>177</v>
-      </c>
-      <c r="C124" s="17">
-        <v>-8.1048700733912096</v>
-      </c>
-      <c r="D124" s="21">
-        <v>-34.891163918022997</v>
-      </c>
-      <c r="E124">
-        <v>145</v>
-      </c>
-      <c r="F124">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="22" t="s">
-        <v>225</v>
-      </c>
-      <c r="B125" s="22" t="s">
-        <v>225</v>
-      </c>
-      <c r="C125" s="23">
-        <v>-8.0635997672068793</v>
-      </c>
-      <c r="D125" s="23">
-        <v>-34.881890011734797</v>
-      </c>
-      <c r="F125" s="22">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="B126" s="22" t="s">
-        <v>226</v>
-      </c>
-      <c r="C126" s="24">
-        <v>-8.0297949481864208</v>
-      </c>
-      <c r="D126" s="24">
-        <v>-34.929545690228501</v>
+      <c r="B126" t="s">
+        <v>197</v>
+      </c>
+      <c r="C126" s="13">
+        <v>-8.1129139186695003</v>
+      </c>
+      <c r="D126" s="13">
+        <v>-34.892622764508502</v>
+      </c>
+      <c r="E126">
+        <v>148</v>
+      </c>
+      <c r="F126">
+        <v>1</v>
+      </c>
+      <c r="G126" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A127" s="5" t="s">
-        <v>179</v>
+      <c r="A127" t="s">
+        <v>185</v>
       </c>
       <c r="B127" t="s">
-        <v>199</v>
-      </c>
-      <c r="C127" s="16">
-        <v>-8.1062248248406696</v>
-      </c>
-      <c r="D127" s="16">
-        <v>-34.889176660810698</v>
+        <v>198</v>
+      </c>
+      <c r="C127" s="14">
+        <v>-8.1213842543624306</v>
+      </c>
+      <c r="D127" s="14">
+        <v>-34.896742272749499</v>
+      </c>
+      <c r="E127">
+        <v>149</v>
+      </c>
+      <c r="F127">
+        <v>1</v>
       </c>
       <c r="G127" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A128" t="s">
-        <v>187</v>
-      </c>
-      <c r="B128" t="s">
-        <v>200</v>
-      </c>
-      <c r="C128" s="17">
-        <v>-8.1213842543624306</v>
-      </c>
-      <c r="D128" s="17">
-        <v>-34.896742272749499</v>
+      <c r="A128" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="B128" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="C128" s="14">
+        <v>-8.0951588190898107</v>
+      </c>
+      <c r="D128" s="14">
+        <v>-34.885862444833599</v>
+      </c>
+      <c r="E128">
+        <v>150</v>
+      </c>
+      <c r="F128">
+        <v>2</v>
       </c>
       <c r="G128" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A129" t="s">
+        <v>184</v>
+      </c>
+      <c r="B129" t="s">
+        <v>199</v>
+      </c>
+      <c r="C129" s="13">
+        <v>-8.1234744929365093</v>
+      </c>
+      <c r="D129" s="13">
+        <v>-34.899869662926399</v>
+      </c>
+      <c r="E129">
+        <v>151</v>
+      </c>
+      <c r="F129">
+        <v>1</v>
+      </c>
+      <c r="G129" t="s">
         <v>180</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A129" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="B129" s="22" t="s">
-        <v>219</v>
-      </c>
-      <c r="C129" s="17">
-        <v>-8.0951588190898107</v>
-      </c>
-      <c r="D129" s="17">
-        <v>-34.885862444833599</v>
-      </c>
-      <c r="G129" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B130" t="s">
-        <v>201</v>
-      </c>
-      <c r="C130" s="16">
-        <v>-8.1234744929365093</v>
-      </c>
-      <c r="D130" s="16">
-        <v>-34.899869662926399</v>
+        <v>200</v>
+      </c>
+      <c r="C130" s="15">
+        <v>-8.1316445036234501</v>
+      </c>
+      <c r="D130" s="15">
+        <v>-34.902758621825001</v>
+      </c>
+      <c r="E130">
+        <v>152</v>
+      </c>
+      <c r="F130">
+        <v>2</v>
       </c>
       <c r="G130" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B131" t="s">
         <v>202</v>
       </c>
-      <c r="C131" s="18">
-        <v>-8.1316445036234501</v>
-      </c>
-      <c r="D131" s="18">
-        <v>-34.902758621825001</v>
+      <c r="C131" s="15">
+        <v>-8.1443519397406607</v>
+      </c>
+      <c r="D131" s="15">
+        <v>-34.906480195132502</v>
+      </c>
+      <c r="E131">
+        <v>153</v>
+      </c>
+      <c r="F131">
+        <v>1</v>
       </c>
       <c r="G131" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A132" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="B132" t="s">
+        <v>201</v>
+      </c>
+      <c r="C132" s="14">
+        <v>-8.1357574755544597</v>
+      </c>
+      <c r="D132" s="14">
+        <v>-34.908424559020403</v>
+      </c>
+      <c r="E132">
+        <v>154</v>
+      </c>
+      <c r="F132">
+        <v>2</v>
+      </c>
+      <c r="G132" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A132" t="s">
-        <v>190</v>
-      </c>
-      <c r="B132" t="s">
-        <v>204</v>
-      </c>
-      <c r="C132" s="18">
-        <v>-8.1443519397406607</v>
-      </c>
-      <c r="D132" s="18">
-        <v>-34.906480195132502</v>
-      </c>
-      <c r="G132" t="s">
-        <v>184</v>
-      </c>
-    </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A133" s="4" t="s">
-        <v>191</v>
+      <c r="A133" t="s">
+        <v>194</v>
       </c>
       <c r="B133" t="s">
-        <v>203</v>
-      </c>
-      <c r="C133" s="17">
-        <v>-8.1357574755544597</v>
-      </c>
-      <c r="D133" s="17">
-        <v>-34.908424559020403</v>
+        <v>205</v>
+      </c>
+      <c r="C133" s="13">
+        <v>-8.0682650000000002</v>
+      </c>
+      <c r="D133" s="13">
+        <v>-34.909804999999999</v>
+      </c>
+      <c r="E133">
+        <v>155</v>
+      </c>
+      <c r="F133">
+        <v>1</v>
       </c>
       <c r="G133" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="B134" t="s">
-        <v>207</v>
-      </c>
-      <c r="C134" s="16">
-        <v>-8.0682650000000002</v>
-      </c>
-      <c r="D134" s="16">
-        <v>-34.909804999999999</v>
+        <v>206</v>
+      </c>
+      <c r="C134" s="13">
+        <v>-8.0577959999999997</v>
+      </c>
+      <c r="D134" s="13">
+        <v>-34.883166000000003</v>
+      </c>
+      <c r="E134">
+        <v>156</v>
+      </c>
+      <c r="F134">
+        <v>1</v>
       </c>
       <c r="G134" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="B135" t="s">
         <v>208</v>
       </c>
-      <c r="C135" s="16">
-        <v>-8.0577959999999997</v>
-      </c>
-      <c r="D135" s="16">
-        <v>-34.883166000000003</v>
+      <c r="C135" s="13">
+        <v>-8.0451259999999998</v>
+      </c>
+      <c r="D135" s="13">
+        <v>-34.902045999999999</v>
+      </c>
+      <c r="E135">
+        <v>157</v>
+      </c>
+      <c r="F135">
+        <v>1</v>
       </c>
       <c r="G135" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A136" t="s">
-        <v>197</v>
-      </c>
-      <c r="B136" t="s">
+      <c r="A136" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="B136" s="18" t="s">
         <v>210</v>
       </c>
-      <c r="C136" s="16">
-        <v>-8.0451259999999998</v>
-      </c>
-      <c r="D136" s="16">
-        <v>-34.902045999999999</v>
+      <c r="C136" s="13">
+        <v>-8.0595918660612593</v>
+      </c>
+      <c r="D136" s="13">
+        <v>-34.886419614608201</v>
+      </c>
+      <c r="E136">
+        <v>158</v>
+      </c>
+      <c r="F136">
+        <v>1</v>
       </c>
       <c r="G136" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A137" t="s">
+        <v>211</v>
+      </c>
+      <c r="B137" t="s">
+        <v>212</v>
+      </c>
+      <c r="C137" s="13">
+        <v>-8.0239212086655201</v>
+      </c>
+      <c r="D137" s="13">
+        <v>-34.897226975193099</v>
+      </c>
+      <c r="E137">
+        <v>159</v>
+      </c>
+      <c r="F137">
+        <v>1</v>
+      </c>
+      <c r="G137" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A137" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="B137" s="22" t="s">
-        <v>212</v>
-      </c>
-      <c r="C137" s="16">
-        <v>-8.0595918660612593</v>
-      </c>
-      <c r="D137" s="16">
-        <v>-34.886419614608201</v>
-      </c>
-      <c r="G137" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
@@ -3920,79 +3999,103 @@
       <c r="B138" t="s">
         <v>214</v>
       </c>
-      <c r="C138" s="16">
-        <v>-8.0239212086655201</v>
-      </c>
-      <c r="D138" s="16">
-        <v>-34.897226975193099</v>
+      <c r="C138" s="13">
+        <v>-8.0313044697048603</v>
+      </c>
+      <c r="D138" s="13">
+        <v>-34.902172963415303</v>
+      </c>
+      <c r="E138">
+        <v>160</v>
+      </c>
+      <c r="F138">
+        <v>1</v>
       </c>
       <c r="G138" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
+        <v>216</v>
+      </c>
+      <c r="B139" t="s">
         <v>215</v>
       </c>
-      <c r="B139" t="s">
-        <v>216</v>
-      </c>
-      <c r="C139" s="16">
-        <v>-8.0313044697048603</v>
-      </c>
-      <c r="D139" s="16">
-        <v>-34.902172963415303</v>
+      <c r="C139" s="13">
+        <v>-8.0990571360815995</v>
+      </c>
+      <c r="D139" s="13">
+        <v>-34.885838700681703</v>
+      </c>
+      <c r="E139">
+        <v>161</v>
+      </c>
+      <c r="F139">
+        <v>2</v>
       </c>
       <c r="G139" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B140" t="s">
-        <v>217</v>
-      </c>
-      <c r="C140" s="16">
-        <v>-8.0990571360815995</v>
-      </c>
-      <c r="D140" s="16">
-        <v>-34.885838700681703</v>
+        <v>220</v>
+      </c>
+      <c r="C140" s="13">
+        <v>-8.1162072256009594</v>
+      </c>
+      <c r="D140" s="13">
+        <v>-34.894632005796097</v>
+      </c>
+      <c r="E140">
+        <v>162</v>
+      </c>
+      <c r="F140">
+        <v>1</v>
       </c>
       <c r="G140" t="s">
-        <v>198</v>
+        <v>219</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="B141" t="s">
-        <v>222</v>
-      </c>
-      <c r="C141" s="16">
+        <v>220</v>
+      </c>
+      <c r="C141" s="13">
         <v>-8.1162072256009594</v>
       </c>
-      <c r="D141" s="16">
+      <c r="D141" s="13">
         <v>-34.894632005796097</v>
       </c>
+      <c r="E141">
+        <v>163</v>
+      </c>
+      <c r="F141">
+        <v>1</v>
+      </c>
       <c r="G141" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D142" s="9"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C143" s="19"/>
+      <c r="C143" s="16"/>
       <c r="D143" s="9"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D144" s="9"/>
     </row>
     <row r="145" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C145" s="20"/>
+      <c r="C145" s="17"/>
       <c r="D145" s="9"/>
     </row>
     <row r="146" spans="3:4" x14ac:dyDescent="0.3">
@@ -4005,7 +4108,7 @@
       <c r="D148" s="9"/>
     </row>
     <row r="149" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C149" s="19"/>
+      <c r="C149" s="16"/>
       <c r="D149" s="9"/>
     </row>
     <row r="150" spans="3:4" x14ac:dyDescent="0.3">
@@ -4015,21 +4118,21 @@
       <c r="D151" s="9"/>
     </row>
     <row r="152" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C152" s="19"/>
+      <c r="C152" s="16"/>
       <c r="D152" s="9"/>
     </row>
     <row r="153" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D153" s="9"/>
     </row>
     <row r="154" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C154" s="19"/>
+      <c r="C154" s="16"/>
       <c r="D154" s="9"/>
     </row>
     <row r="155" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D155" s="9"/>
     </row>
     <row r="156" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C156" s="20"/>
+      <c r="C156" s="17"/>
       <c r="D156" s="9"/>
     </row>
     <row r="157" spans="3:4" x14ac:dyDescent="0.3">
@@ -4063,11 +4166,11 @@
       <c r="D166" s="9"/>
     </row>
     <row r="167" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C167" s="20"/>
+      <c r="C167" s="17"/>
       <c r="D167" s="9"/>
     </row>
     <row r="168" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C168" s="20"/>
+      <c r="C168" s="17"/>
       <c r="D168" s="9"/>
     </row>
     <row r="169" spans="3:4" x14ac:dyDescent="0.3">
@@ -4497,7 +4600,8 @@
       <c r="D676" s="9"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <autoFilter ref="A1:F141" xr:uid="{22014C47-1C13-4AB1-9850-A592523522E1}"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -4520,191 +4624,191 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C2" t="s">
-        <v>199</v>
-      </c>
-      <c r="D2" s="16">
+        <v>197</v>
+      </c>
+      <c r="D2" s="13">
         <v>-8.1062248248406696</v>
       </c>
-      <c r="E2" s="16">
+      <c r="E2" s="13">
         <v>-34.889176660810698</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B3" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C3" t="s">
-        <v>200</v>
-      </c>
-      <c r="D3" s="17">
+        <v>198</v>
+      </c>
+      <c r="D3" s="14">
         <v>-8.1213842543624306</v>
       </c>
-      <c r="E3" s="17">
+      <c r="E3" s="14">
         <v>-34.896742272749499</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>181</v>
-      </c>
-      <c r="B4" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>219</v>
-      </c>
-      <c r="D4" s="17">
+        <v>179</v>
+      </c>
+      <c r="B4" s="18" t="s">
+        <v>184</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>217</v>
+      </c>
+      <c r="D4" s="14">
         <v>-8095158819089810</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>220</v>
+      <c r="E4" s="14" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D5" s="16">
+        <v>199</v>
+      </c>
+      <c r="D5" s="13">
         <v>-8.1234744929365093</v>
       </c>
-      <c r="E5" s="16">
+      <c r="E5" s="13">
         <v>-34.899869662926399</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C6" t="s">
-        <v>202</v>
-      </c>
-      <c r="D6" s="18">
+        <v>200</v>
+      </c>
+      <c r="D6" s="15">
         <v>-8131644503623450</v>
       </c>
-      <c r="E6" s="18">
+      <c r="E6" s="15">
         <v>-3490275862182500</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C7" t="s">
-        <v>204</v>
-      </c>
-      <c r="D7" s="18">
+        <v>202</v>
+      </c>
+      <c r="D7" s="15">
         <v>-8.1443519397406607</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="15">
         <v>-34.906480195132502</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C8" t="s">
-        <v>203</v>
-      </c>
-      <c r="D8" s="17">
+        <v>201</v>
+      </c>
+      <c r="D8" s="14">
         <v>-8.1357574755544597</v>
       </c>
-      <c r="E8" s="17">
+      <c r="E8" s="14">
         <v>-34.908424559020403</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C9" t="s">
-        <v>207</v>
-      </c>
-      <c r="D9" s="16">
+        <v>205</v>
+      </c>
+      <c r="D9" s="13">
         <v>-8.0682650000000002</v>
       </c>
-      <c r="E9" s="16">
+      <c r="E9" s="13">
         <v>-34.909804999999999</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B10" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C10" t="s">
-        <v>208</v>
-      </c>
-      <c r="D10" s="16">
+        <v>206</v>
+      </c>
+      <c r="D10" s="13">
         <v>-8.0577959999999997</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="13">
         <v>-34.883166000000003</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B11" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C11" t="s">
-        <v>210</v>
-      </c>
-      <c r="D11" s="16">
+        <v>208</v>
+      </c>
+      <c r="D11" s="13">
         <v>-8.0451259999999998</v>
       </c>
-      <c r="E11" s="16">
+      <c r="E11" s="13">
         <v>-34.902045999999999</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>193</v>
-      </c>
-      <c r="B12" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="C12" s="22" t="s">
-        <v>212</v>
+        <v>191</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>209</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>210</v>
       </c>
       <c r="D12" s="1">
         <v>-8059591866061260</v>
@@ -4715,13 +4819,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B13" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C13" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D13" s="1">
         <v>-8023921208665520</v>
@@ -4732,13 +4836,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B14" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C14" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D14" s="1">
         <v>-8031304469704860</v>
@@ -4749,13 +4853,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="B15" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C15" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="D15" s="1">
         <v>-8099057136081600</v>
@@ -4766,13 +4870,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B16" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C16" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D16" s="1">
         <v>-8116207225600960</v>
@@ -4788,7 +4892,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="4" type="noConversion"/>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
atualizando quantitativo de câmeras dos pontos mínimos.
</commit_message>
<xml_diff>
--- a/data/Prioridades.xlsx
+++ b/data/Prioridades.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Consultor\OneDrive - Aquila\Área de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Consultor\Desktop\COP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8860369-639D-4094-95A9-2076E546D450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DC325D-F227-4806-A7E0-05F75E5AA309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{397ABB56-F0FE-4E29-B5CB-823307B18FC8}"/>
   </bookViews>
@@ -1203,7 +1203,7 @@
   <dimension ref="A1:G676"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F134" sqref="F134"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1253,7 +1253,7 @@
         <v>7</v>
       </c>
       <c r="F2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
ajustando nome das vias prioritárias.
</commit_message>
<xml_diff>
--- a/data/Prioridades.xlsx
+++ b/data/Prioridades.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Consultor\Desktop\COP\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Consultor\OneDrive - Aquila\Área de Trabalho\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DC325D-F227-4806-A7E0-05F75E5AA309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D86E76D2-A606-444F-813D-C55433335D4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{397ABB56-F0FE-4E29-B5CB-823307B18FC8}"/>
   </bookViews>
@@ -38,7 +38,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="227">
+  <si>
+    <t>LATITUDE COM PONTO</t>
+  </si>
+  <si>
+    <t>LONGITUDE COM PONTO</t>
+  </si>
   <si>
     <t>AVENIDA CAXANGA</t>
   </si>
@@ -713,12 +719,6 @@
   </si>
   <si>
     <t>Ponte Engenheiro jaime Gusmão</t>
-  </si>
-  <si>
-    <t>lat</t>
-  </si>
-  <si>
-    <t>log</t>
   </si>
 </sst>
 </file>
@@ -727,10 +727,10 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.00000"/>
-    <numFmt numFmtId="165" formatCode="#,##0.000000"/>
-    <numFmt numFmtId="166" formatCode="0.000000"/>
+    <numFmt numFmtId="169" formatCode="#,##0.000000"/>
+    <numFmt numFmtId="177" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -753,6 +753,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -763,20 +771,6 @@
       <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="7"/>
-      <color rgb="FF007B8B"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="4" tint="-0.499984740745262"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="6">
@@ -838,7 +832,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -856,36 +850,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="169" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="177" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1203,7 +1194,7 @@
   <dimension ref="A1:G676"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1218,55 +1209,55 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C1" t="s">
-        <v>225</v>
+        <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>226</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="F1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
-      </c>
-      <c r="C2" s="13">
+        <v>121</v>
+      </c>
+      <c r="C2">
         <v>-8.0625199999999992</v>
       </c>
-      <c r="D2" s="13">
+      <c r="D2">
         <v>-34.931939999999997</v>
       </c>
       <c r="E2">
         <v>7</v>
       </c>
       <c r="F2">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>134</v>
-      </c>
-      <c r="C3" s="13">
+        <v>136</v>
+      </c>
+      <c r="C3">
         <v>-8.0349699999999995</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3">
         <v>-34.949379999999998</v>
       </c>
       <c r="E3">
@@ -1278,15 +1269,15 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" t="s">
         <v>126</v>
       </c>
-      <c r="B4" t="s">
-        <v>124</v>
-      </c>
-      <c r="C4" s="13">
+      <c r="C4">
         <v>-8.0387400000000007</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4">
         <v>-34.942459999999997</v>
       </c>
       <c r="E4">
@@ -1298,15 +1289,15 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>135</v>
-      </c>
-      <c r="C5" s="13">
+        <v>137</v>
+      </c>
+      <c r="C5">
         <v>-8.0782500000000006</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5">
         <v>-34.909379999999999</v>
       </c>
       <c r="E5">
@@ -1318,15 +1309,15 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="C6" s="13">
+        <v>139</v>
+      </c>
+      <c r="C6">
         <v>-8.0895499999999991</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6">
         <v>-34.882910000000003</v>
       </c>
       <c r="E6">
@@ -1338,15 +1329,15 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="C7" s="13">
+        <v>142</v>
+      </c>
+      <c r="C7">
         <v>-8.11951</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7">
         <v>-34.896729999999998</v>
       </c>
       <c r="E7">
@@ -1358,15 +1349,15 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" s="13">
+        <v>132</v>
+      </c>
+      <c r="C8">
         <v>-8.0474399999999999</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8">
         <v>-34.876989999999999</v>
       </c>
       <c r="E8">
@@ -1378,15 +1369,15 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
-      </c>
-      <c r="C9" s="13">
+        <v>131</v>
+      </c>
+      <c r="C9">
         <v>-8.0848800000000001</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9">
         <v>-34.928669999999997</v>
       </c>
       <c r="E9">
@@ -1398,15 +1389,15 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B10" t="s">
-        <v>121</v>
-      </c>
-      <c r="C10" s="13">
+        <v>123</v>
+      </c>
+      <c r="C10">
         <v>-8.1367899999999995</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10">
         <v>-34.916919999999998</v>
       </c>
       <c r="E10">
@@ -1418,35 +1409,35 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B11" t="s">
-        <v>121</v>
-      </c>
-      <c r="C11" s="13">
+        <v>123</v>
+      </c>
+      <c r="C11">
         <v>-8.1222300000000001</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11">
         <v>-34.914400000000001</v>
       </c>
       <c r="E11">
         <v>35</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B12" t="s">
-        <v>121</v>
-      </c>
-      <c r="C12" s="13">
+        <v>123</v>
+      </c>
+      <c r="C12">
         <v>-8.1186299999999996</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12">
         <v>-34.913719999999998</v>
       </c>
       <c r="E12">
@@ -1458,15 +1449,15 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B13" t="s">
-        <v>121</v>
-      </c>
-      <c r="C13" s="13">
+        <v>123</v>
+      </c>
+      <c r="C13">
         <v>-8.1115499999999994</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D13">
         <v>-34.91234</v>
       </c>
       <c r="E13">
@@ -1478,15 +1469,15 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>126</v>
-      </c>
-      <c r="B14" t="s">
-        <v>121</v>
-      </c>
-      <c r="C14" s="13">
+        <v>128</v>
+      </c>
+      <c r="B14" s="23" t="s">
+        <v>123</v>
+      </c>
+      <c r="C14">
         <v>-8.1089400000000005</v>
       </c>
-      <c r="D14" s="13">
+      <c r="D14">
         <v>-34.911799999999999</v>
       </c>
       <c r="E14">
@@ -1498,15 +1489,15 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B15" t="s">
-        <v>121</v>
-      </c>
-      <c r="C15" s="13">
+        <v>123</v>
+      </c>
+      <c r="C15">
         <v>-8.1061999999999994</v>
       </c>
-      <c r="D15" s="13">
+      <c r="D15">
         <v>-34.911259999999999</v>
       </c>
       <c r="E15">
@@ -1518,15 +1509,15 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B16" t="s">
-        <v>117</v>
-      </c>
-      <c r="C16" s="13">
+        <v>119</v>
+      </c>
+      <c r="C16">
         <v>-8.0472400000000004</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16">
         <v>-34.891530000000003</v>
       </c>
       <c r="E16">
@@ -1538,15 +1529,15 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
-      </c>
-      <c r="C17" s="13">
+        <v>119</v>
+      </c>
+      <c r="C17">
         <v>-8.0501900000000006</v>
       </c>
-      <c r="D17" s="13">
+      <c r="D17">
         <v>-34.894350000000003</v>
       </c>
       <c r="E17">
@@ -1558,35 +1549,35 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B18" t="s">
-        <v>117</v>
-      </c>
-      <c r="C18" s="13">
+        <v>119</v>
+      </c>
+      <c r="C18">
         <v>-8.0502800000000008</v>
       </c>
-      <c r="D18" s="13">
+      <c r="D18">
         <v>-34.893889999999999</v>
       </c>
       <c r="E18">
         <v>3</v>
       </c>
       <c r="F18">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B19" t="s">
-        <v>117</v>
-      </c>
-      <c r="C19" s="13">
+        <v>119</v>
+      </c>
+      <c r="C19">
         <v>-8.0542800000000003</v>
       </c>
-      <c r="D19" s="13">
+      <c r="D19">
         <v>-34.896850000000001</v>
       </c>
       <c r="E19">
@@ -1598,15 +1589,15 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
-      </c>
-      <c r="C20" s="13">
+        <v>119</v>
+      </c>
+      <c r="C20">
         <v>-8.0571900000000003</v>
       </c>
-      <c r="D20" s="13">
+      <c r="D20">
         <v>-34.898229999999998</v>
       </c>
       <c r="E20">
@@ -1618,15 +1609,15 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="C21" s="13">
+        <v>138</v>
+      </c>
+      <c r="C21">
         <v>-8.0796600000000005</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21">
         <v>-34.93374</v>
       </c>
       <c r="E21">
@@ -1638,15 +1629,15 @@
     </row>
     <row r="22" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="C22" s="13">
+        <v>124</v>
+      </c>
+      <c r="C22" s="7">
         <v>-8.1066699999999994</v>
       </c>
-      <c r="D22" s="13">
+      <c r="D22" s="7">
         <v>-34.927349999999997</v>
       </c>
       <c r="E22" s="7">
@@ -1658,15 +1649,15 @@
     </row>
     <row r="23" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="C23" s="13">
+        <v>124</v>
+      </c>
+      <c r="C23" s="7">
         <v>-8.1077700000000004</v>
       </c>
-      <c r="D23" s="13">
+      <c r="D23" s="7">
         <v>-34.927169999999997</v>
       </c>
       <c r="E23" s="7">
@@ -1678,15 +1669,15 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B24" t="s">
-        <v>125</v>
-      </c>
-      <c r="C24" s="13">
+        <v>127</v>
+      </c>
+      <c r="C24">
         <v>-8.0779700000000005</v>
       </c>
-      <c r="D24" s="13">
+      <c r="D24">
         <v>-34.89781</v>
       </c>
       <c r="E24">
@@ -1698,15 +1689,15 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>133</v>
-      </c>
-      <c r="C25" s="13">
+        <v>135</v>
+      </c>
+      <c r="C25">
         <v>-8.0017399999999999</v>
       </c>
-      <c r="D25" s="13">
+      <c r="D25">
         <v>-34.923749999999998</v>
       </c>
       <c r="E25">
@@ -1718,15 +1709,15 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="C26" s="13">
+        <v>134</v>
+      </c>
+      <c r="C26">
         <v>-8.0254999999999992</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26">
         <v>-34.906619999999997</v>
       </c>
       <c r="E26">
@@ -1738,15 +1729,15 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B27" t="s">
-        <v>127</v>
-      </c>
-      <c r="C27" s="13">
+        <v>129</v>
+      </c>
+      <c r="C27">
         <v>-8.0549599999999995</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D27">
         <v>-34.895820000000001</v>
       </c>
       <c r="E27">
@@ -1758,15 +1749,15 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="C28" s="13">
+        <v>133</v>
+      </c>
+      <c r="C28">
         <v>-8.0661900000000006</v>
       </c>
-      <c r="D28" s="13">
+      <c r="D28">
         <v>-34.889449999999997</v>
       </c>
       <c r="E28">
@@ -1778,15 +1769,15 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B29" t="s">
-        <v>120</v>
-      </c>
-      <c r="C29" s="13">
+        <v>122</v>
+      </c>
+      <c r="C29">
         <v>-8.0796600000000005</v>
       </c>
-      <c r="D29" s="13">
+      <c r="D29">
         <v>-34.904530000000001</v>
       </c>
       <c r="E29">
@@ -1798,15 +1789,15 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B30" t="s">
-        <v>128</v>
-      </c>
-      <c r="C30" s="13">
+        <v>130</v>
+      </c>
+      <c r="C30">
         <v>-8.0782000000000007</v>
       </c>
-      <c r="D30" s="13">
+      <c r="D30">
         <v>-34.905520000000003</v>
       </c>
       <c r="E30">
@@ -1818,15 +1809,15 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="C31" s="13">
+        <v>140</v>
+      </c>
+      <c r="C31">
         <v>-8.1105800000000006</v>
       </c>
-      <c r="D31" s="13">
+      <c r="D31">
         <v>-34.937100000000001</v>
       </c>
       <c r="E31">
@@ -1838,15 +1829,15 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>139</v>
-      </c>
-      <c r="C32" s="13">
+        <v>141</v>
+      </c>
+      <c r="C32">
         <v>-8.1229300000000002</v>
       </c>
-      <c r="D32" s="13">
+      <c r="D32">
         <v>-34.903959999999998</v>
       </c>
       <c r="E32">
@@ -1858,15 +1849,15 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B33" t="s">
-        <v>123</v>
-      </c>
-      <c r="C33" s="13">
+        <v>125</v>
+      </c>
+      <c r="C33">
         <v>-8.1418700000000008</v>
       </c>
-      <c r="D33" s="13">
+      <c r="D33">
         <v>-34.918700000000001</v>
       </c>
       <c r="E33">
@@ -1878,15 +1869,15 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B34" t="s">
-        <v>79</v>
-      </c>
-      <c r="C34" s="13">
+        <v>81</v>
+      </c>
+      <c r="C34" s="11">
         <v>-8.0629100000000005</v>
       </c>
-      <c r="D34" s="13">
+      <c r="D34" s="11">
         <v>-34.871960000000001</v>
       </c>
       <c r="E34">
@@ -1898,15 +1889,15 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B35" t="s">
-        <v>143</v>
-      </c>
-      <c r="C35" s="13">
+        <v>145</v>
+      </c>
+      <c r="C35" s="11">
         <v>-8.0658437972273997</v>
       </c>
-      <c r="D35" s="13">
+      <c r="D35" s="11">
         <v>-34.879644548383098</v>
       </c>
       <c r="E35">
@@ -1918,16 +1909,16 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B36" t="s">
-        <v>82</v>
-      </c>
-      <c r="C36" s="13">
-        <v>-8.0596910799380197</v>
-      </c>
-      <c r="D36" s="13">
-        <v>-34.869988064354096</v>
+        <v>84</v>
+      </c>
+      <c r="C36">
+        <v>-8.0652100000000004</v>
+      </c>
+      <c r="D36">
+        <v>-34.876049999999999</v>
       </c>
       <c r="E36">
         <v>42</v>
@@ -1937,16 +1928,16 @@
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A37" s="11" t="s">
-        <v>145</v>
+      <c r="A37" s="12" t="s">
+        <v>147</v>
       </c>
       <c r="B37" t="s">
-        <v>57</v>
-      </c>
-      <c r="C37" s="13">
+        <v>59</v>
+      </c>
+      <c r="C37" s="11">
         <v>-8.0561880640993202</v>
       </c>
-      <c r="D37" s="13">
+      <c r="D37" s="11">
         <v>-34.877104862147597</v>
       </c>
       <c r="E37">
@@ -1958,15 +1949,15 @@
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B38" t="s">
-        <v>23</v>
-      </c>
-      <c r="C38" s="13">
+        <v>25</v>
+      </c>
+      <c r="C38" s="11">
         <v>-8.031604626120016</v>
       </c>
-      <c r="D38" s="13">
+      <c r="D38" s="11">
         <v>-34.924639637975957</v>
       </c>
       <c r="E38">
@@ -1978,15 +1969,15 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B39" t="s">
-        <v>77</v>
-      </c>
-      <c r="C39" s="13">
+        <v>79</v>
+      </c>
+      <c r="C39" s="8">
         <v>-8.0631233071071193</v>
       </c>
-      <c r="D39" s="13">
+      <c r="D39" s="9">
         <v>-34.8710022666098</v>
       </c>
       <c r="E39">
@@ -1998,15 +1989,15 @@
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B40" t="s">
-        <v>89</v>
-      </c>
-      <c r="C40" s="13">
+        <v>91</v>
+      </c>
+      <c r="C40">
         <v>-8.0632113000000007</v>
       </c>
-      <c r="D40" s="13">
+      <c r="D40">
         <v>-34.891190299999998</v>
       </c>
       <c r="E40">
@@ -2018,15 +2009,15 @@
     </row>
     <row r="41" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C41" s="13">
+        <v>20</v>
+      </c>
+      <c r="C41" s="4">
         <v>-8.0373614419372608</v>
       </c>
-      <c r="D41" s="13">
+      <c r="D41" s="4">
         <v>-34.892167160062002</v>
       </c>
       <c r="E41" s="4">
@@ -2038,15 +2029,15 @@
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B42" t="s">
-        <v>33</v>
-      </c>
-      <c r="C42" s="13">
+        <v>35</v>
+      </c>
+      <c r="C42">
         <v>-8.0523349999999994</v>
       </c>
-      <c r="D42" s="13">
+      <c r="D42">
         <v>-34.908380000000001</v>
       </c>
       <c r="E42">
@@ -2058,15 +2049,15 @@
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B43" t="s">
-        <v>109</v>
-      </c>
-      <c r="C43" s="13">
+        <v>111</v>
+      </c>
+      <c r="C43">
         <v>-8.0443764000000009</v>
       </c>
-      <c r="D43" s="13">
+      <c r="D43">
         <v>-34.910375999999999</v>
       </c>
       <c r="E43">
@@ -2078,15 +2069,15 @@
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B44" t="s">
-        <v>91</v>
-      </c>
-      <c r="C44" s="13">
+        <v>93</v>
+      </c>
+      <c r="C44">
         <v>-8.0710313649999996</v>
       </c>
-      <c r="D44" s="13">
+      <c r="D44">
         <v>-34.877230730000001</v>
       </c>
       <c r="E44">
@@ -2098,15 +2089,15 @@
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B45" t="s">
-        <v>128</v>
-      </c>
-      <c r="C45" s="13">
+        <v>130</v>
+      </c>
+      <c r="C45">
         <v>-8.0774484770977697</v>
       </c>
-      <c r="D45" s="13">
+      <c r="D45">
         <v>-34.906173347262097</v>
       </c>
       <c r="E45">
@@ -2118,15 +2109,15 @@
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B46" t="s">
-        <v>108</v>
-      </c>
-      <c r="C46" s="13">
+        <v>110</v>
+      </c>
+      <c r="C46">
         <v>-8.019325791</v>
       </c>
-      <c r="D46" s="13">
+      <c r="D46">
         <v>-34.893893419999998</v>
       </c>
       <c r="E46">
@@ -2138,15 +2129,15 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B47" t="s">
-        <v>107</v>
-      </c>
-      <c r="C47" s="13">
+        <v>109</v>
+      </c>
+      <c r="C47">
         <v>-8.0026340841323993</v>
       </c>
-      <c r="D47" s="13">
+      <c r="D47">
         <v>-34.897381311996803</v>
       </c>
       <c r="E47">
@@ -2158,15 +2149,15 @@
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B48" t="s">
-        <v>84</v>
-      </c>
-      <c r="C48" s="13">
+        <v>86</v>
+      </c>
+      <c r="C48">
         <v>-8.0262613999999992</v>
       </c>
-      <c r="D48" s="13">
+      <c r="D48">
         <v>-34.920241699999998</v>
       </c>
       <c r="E48">
@@ -2178,15 +2169,15 @@
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B49" t="s">
-        <v>106</v>
-      </c>
-      <c r="C49" s="13">
+        <v>108</v>
+      </c>
+      <c r="C49">
         <v>-8.0466867719999993</v>
       </c>
-      <c r="D49" s="13">
+      <c r="D49">
         <v>-34.876619990000002</v>
       </c>
       <c r="E49">
@@ -2198,15 +2189,15 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B50" t="s">
-        <v>66</v>
-      </c>
-      <c r="C50" s="13">
+        <v>68</v>
+      </c>
+      <c r="C50" s="11">
         <v>-8.0683118247106602</v>
       </c>
-      <c r="D50" s="13">
+      <c r="D50" s="11">
         <v>-34.877617084802701</v>
       </c>
       <c r="E50">
@@ -2218,15 +2209,15 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B51" t="s">
-        <v>1</v>
-      </c>
-      <c r="C51" s="13">
+        <v>3</v>
+      </c>
+      <c r="C51">
         <v>-8.0518440560000002</v>
       </c>
-      <c r="D51" s="13">
+      <c r="D51">
         <v>-34.921453929999998</v>
       </c>
       <c r="E51">
@@ -2238,15 +2229,15 @@
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B52" t="s">
-        <v>110</v>
-      </c>
-      <c r="C52" s="13">
+        <v>112</v>
+      </c>
+      <c r="C52">
         <v>-8.0871689789999994</v>
       </c>
-      <c r="D52" s="13">
+      <c r="D52">
         <v>-34.882869679999999</v>
       </c>
       <c r="E52">
@@ -2258,15 +2249,15 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B53" t="s">
-        <v>40</v>
-      </c>
-      <c r="C53" s="13">
+        <v>42</v>
+      </c>
+      <c r="C53" s="8">
         <v>-8.0918133099417098</v>
       </c>
-      <c r="D53" s="13">
+      <c r="D53" s="9">
         <v>-34.881938263926898</v>
       </c>
       <c r="E53">
@@ -2278,15 +2269,15 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B54" t="s">
-        <v>105</v>
-      </c>
-      <c r="C54" s="13">
+        <v>107</v>
+      </c>
+      <c r="C54" s="11">
         <v>-8.1169846559999996</v>
       </c>
-      <c r="D54" s="13">
+      <c r="D54" s="11">
         <v>-34.912922829999999</v>
       </c>
       <c r="E54">
@@ -2298,15 +2289,15 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B55" t="s">
-        <v>81</v>
-      </c>
-      <c r="C55" s="13">
+        <v>83</v>
+      </c>
+      <c r="C55" s="8">
         <v>-8.0647000000000002</v>
       </c>
-      <c r="D55" s="13">
+      <c r="D55" s="9">
         <v>-34.87379</v>
       </c>
       <c r="E55">
@@ -2318,15 +2309,15 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B56" t="s">
-        <v>151</v>
-      </c>
-      <c r="C56" s="13">
+        <v>153</v>
+      </c>
+      <c r="C56">
         <v>-8.0933499999999992</v>
       </c>
-      <c r="D56" s="13">
+      <c r="D56">
         <v>-34.892569999999999</v>
       </c>
       <c r="E56">
@@ -2338,15 +2329,15 @@
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B57" t="s">
-        <v>14</v>
-      </c>
-      <c r="C57" s="13">
+        <v>16</v>
+      </c>
+      <c r="C57">
         <v>-8.1032904511294284</v>
       </c>
-      <c r="D57" s="13">
+      <c r="D57">
         <v>-34.938219328046898</v>
       </c>
       <c r="E57">
@@ -2358,15 +2349,15 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B58" t="s">
-        <v>11</v>
-      </c>
-      <c r="C58" s="13">
+        <v>13</v>
+      </c>
+      <c r="C58" s="11">
         <v>-8.0571900000000003</v>
       </c>
-      <c r="D58" s="13">
+      <c r="D58" s="11">
         <v>-34.943100000000001</v>
       </c>
       <c r="E58">
@@ -2378,15 +2369,15 @@
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B59" t="s">
-        <v>28</v>
-      </c>
-      <c r="C59" s="13">
+        <v>30</v>
+      </c>
+      <c r="C59" s="8">
         <v>-8.03037578</v>
       </c>
-      <c r="D59" s="13">
+      <c r="D59" s="9">
         <v>-34.91302219</v>
       </c>
       <c r="E59">
@@ -2398,15 +2389,15 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B60" t="s">
-        <v>17</v>
-      </c>
-      <c r="C60" s="13">
+        <v>19</v>
+      </c>
+      <c r="C60" s="11">
         <v>-8.0152591867061407</v>
       </c>
-      <c r="D60" s="13">
+      <c r="D60" s="11">
         <v>-34.932259581601897</v>
       </c>
       <c r="E60">
@@ -2418,15 +2409,15 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B61" t="s">
-        <v>44</v>
-      </c>
-      <c r="C61" s="13">
+        <v>46</v>
+      </c>
+      <c r="C61" s="11">
         <v>-8.0455253553702306</v>
       </c>
-      <c r="D61" s="13">
+      <c r="D61" s="11">
         <v>-34.902801244642703</v>
       </c>
       <c r="E61">
@@ -2438,15 +2429,15 @@
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B62" t="s">
-        <v>15</v>
-      </c>
-      <c r="C62" s="13">
+        <v>17</v>
+      </c>
+      <c r="C62" s="11">
         <v>-8.0388800000000007</v>
       </c>
-      <c r="D62" s="13">
+      <c r="D62" s="11">
         <v>-34.927500000000002</v>
       </c>
       <c r="E62">
@@ -2458,15 +2449,15 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B63" t="s">
-        <v>83</v>
-      </c>
-      <c r="C63" s="13">
+        <v>85</v>
+      </c>
+      <c r="C63" s="11">
         <v>-8.0133542866917402</v>
       </c>
-      <c r="D63" s="13">
+      <c r="D63" s="11">
         <v>-34.944212082769504</v>
       </c>
       <c r="E63">
@@ -2478,15 +2469,15 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="C64" s="13">
+        <v>156</v>
+      </c>
+      <c r="C64">
         <v>-8.0757700000000003</v>
       </c>
-      <c r="D64" s="13">
+      <c r="D64">
         <v>-34.889209999999999</v>
       </c>
       <c r="E64">
@@ -2498,15 +2489,15 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B65" t="s">
-        <v>156</v>
-      </c>
-      <c r="C65" s="13">
+        <v>158</v>
+      </c>
+      <c r="C65">
         <v>-8.0682399999999994</v>
       </c>
-      <c r="D65" s="13">
+      <c r="D65">
         <v>-34.893129999999999</v>
       </c>
       <c r="E65">
@@ -2518,15 +2509,15 @@
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B66" t="s">
-        <v>61</v>
-      </c>
-      <c r="C66" s="13">
+        <v>63</v>
+      </c>
+      <c r="C66">
         <v>-8.0568018479999992</v>
       </c>
-      <c r="D66" s="13">
+      <c r="D66">
         <v>-34.881540399999999</v>
       </c>
       <c r="E66">
@@ -2538,15 +2529,15 @@
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>10</v>
-      </c>
-      <c r="C67" s="13">
+        <v>12</v>
+      </c>
+      <c r="C67">
         <v>-8.0670076769999994</v>
       </c>
-      <c r="D67" s="13">
+      <c r="D67">
         <v>-34.878943710000001</v>
       </c>
       <c r="E67">
@@ -2558,15 +2549,15 @@
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B68" t="s">
-        <v>70</v>
-      </c>
-      <c r="C68" s="13">
+        <v>72</v>
+      </c>
+      <c r="C68" s="11">
         <v>-8.0671258986764194</v>
       </c>
-      <c r="D68" s="13">
+      <c r="D68" s="11">
         <v>-34.878057535739302</v>
       </c>
       <c r="E68">
@@ -2578,15 +2569,15 @@
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B69" t="s">
-        <v>108</v>
-      </c>
-      <c r="C69" s="13">
+        <v>110</v>
+      </c>
+      <c r="C69" s="8">
         <v>-8.0030395589999994</v>
       </c>
-      <c r="D69" s="13">
+      <c r="D69" s="9">
         <v>-34.897848570000001</v>
       </c>
       <c r="E69">
@@ -2598,15 +2589,15 @@
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B70" t="s">
-        <v>40</v>
-      </c>
-      <c r="C70" s="13">
+        <v>42</v>
+      </c>
+      <c r="C70" s="8">
         <v>-8.1059000000000001</v>
       </c>
-      <c r="D70" s="13">
+      <c r="D70" s="9">
         <v>-34.887700000000002</v>
       </c>
       <c r="E70">
@@ -2618,16 +2609,16 @@
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B71" t="s">
-        <v>40</v>
-      </c>
-      <c r="C71" s="19">
-        <v>-8108306</v>
-      </c>
-      <c r="D71" s="19">
-        <v>-34888487</v>
+        <v>42</v>
+      </c>
+      <c r="C71" s="8">
+        <v>-8.10501</v>
+      </c>
+      <c r="D71" s="9">
+        <v>-34.887</v>
       </c>
       <c r="E71">
         <v>89</v>
@@ -2638,10 +2629,10 @@
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B72" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C72" s="8">
         <v>-8.1020699999999994</v>
@@ -2658,10 +2649,10 @@
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B73" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C73">
         <v>-8.0354030999999999</v>
@@ -2677,16 +2668,16 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A74" s="4" t="s">
-        <v>34</v>
+      <c r="A74" t="s">
+        <v>36</v>
       </c>
       <c r="B74" t="s">
-        <v>35</v>
-      </c>
-      <c r="C74" s="20">
+        <v>37</v>
+      </c>
+      <c r="C74" s="11">
         <v>-8.0029137349999999</v>
       </c>
-      <c r="D74" s="20">
+      <c r="D74" s="11">
         <v>-34.907381350000001</v>
       </c>
       <c r="E74">
@@ -2697,11 +2688,11 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
-        <v>4</v>
+      <c r="A75" t="s">
+        <v>6</v>
       </c>
       <c r="B75" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C75">
         <v>-8.0917032715727704</v>
@@ -2718,10 +2709,10 @@
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B76" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C76" s="8">
         <v>-8.054316900326878</v>
@@ -2738,15 +2729,15 @@
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B77" t="s">
-        <v>38</v>
-      </c>
-      <c r="C77" s="20">
+        <v>40</v>
+      </c>
+      <c r="C77" s="11">
         <v>-8.0506795404506857</v>
       </c>
-      <c r="D77" s="20">
+      <c r="D77" s="11">
         <v>-34.907087309499254</v>
       </c>
       <c r="E77">
@@ -2758,10 +2749,10 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B78" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C78">
         <v>-8.1057745109999999</v>
@@ -2778,15 +2769,15 @@
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B79" t="s">
-        <v>8</v>
-      </c>
-      <c r="C79" s="20">
+        <v>10</v>
+      </c>
+      <c r="C79" s="11">
         <v>-8.1209634325435704</v>
       </c>
-      <c r="D79" s="20">
+      <c r="D79" s="11">
         <v>-34.945930972484199</v>
       </c>
       <c r="E79">
@@ -2798,10 +2789,10 @@
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B80" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C80" s="8">
         <v>-8.0335093116039573</v>
@@ -2818,10 +2809,10 @@
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B81" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C81">
         <v>-8.057972572465788</v>
@@ -2838,10 +2829,10 @@
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B82" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C82">
         <v>-8.0707956549572497</v>
@@ -2858,15 +2849,15 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B83" t="s">
-        <v>68</v>
-      </c>
-      <c r="C83" s="20">
+        <v>70</v>
+      </c>
+      <c r="C83" s="11">
         <v>-8.0609670624366405</v>
       </c>
-      <c r="D83" s="20">
+      <c r="D83" s="11">
         <v>-34.877245681326698</v>
       </c>
       <c r="E83">
@@ -2878,10 +2869,10 @@
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B84" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C84" s="8">
         <v>-8.0491004724083695</v>
@@ -2898,10 +2889,10 @@
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B85" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C85" s="8">
         <v>-8.1183840561139409</v>
@@ -2918,16 +2909,16 @@
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B86" t="s">
-        <v>46</v>
-      </c>
-      <c r="C86" s="21">
-        <v>-8132158</v>
-      </c>
-      <c r="D86" s="1">
-        <v>-34900280</v>
+        <v>48</v>
+      </c>
+      <c r="C86">
+        <v>-8.1318453757380595</v>
+      </c>
+      <c r="D86">
+        <v>-34.899977714417403</v>
       </c>
       <c r="E86">
         <v>109</v>
@@ -2938,15 +2929,15 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B87" t="s">
-        <v>23</v>
-      </c>
-      <c r="C87" s="20">
+        <v>25</v>
+      </c>
+      <c r="C87" s="11">
         <v>-8.0347728739999997</v>
       </c>
-      <c r="D87" s="20">
+      <c r="D87" s="11">
         <v>-34.919505219999998</v>
       </c>
       <c r="E87">
@@ -2958,15 +2949,15 @@
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B88" t="s">
-        <v>3</v>
-      </c>
-      <c r="C88" s="20">
+        <v>5</v>
+      </c>
+      <c r="C88" s="11">
         <v>-8.0610589800000003</v>
       </c>
-      <c r="D88" s="20">
+      <c r="D88" s="11">
         <v>-34.871273469999998</v>
       </c>
       <c r="E88">
@@ -2978,15 +2969,15 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B89" t="s">
-        <v>17</v>
-      </c>
-      <c r="C89" s="20">
+        <v>19</v>
+      </c>
+      <c r="C89" s="11">
         <v>-8.0234482595867505</v>
       </c>
-      <c r="D89" s="20">
+      <c r="D89" s="11">
         <v>-34.914670590409798</v>
       </c>
       <c r="E89">
@@ -2998,15 +2989,15 @@
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B90" t="s">
-        <v>66</v>
-      </c>
-      <c r="C90" s="20">
+        <v>68</v>
+      </c>
+      <c r="C90" s="11">
         <v>-8.0682260813088291</v>
       </c>
-      <c r="D90" s="20">
+      <c r="D90" s="11">
         <v>-34.878422989818198</v>
       </c>
       <c r="E90">
@@ -3018,19 +3009,19 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="B91" t="s">
-        <v>36</v>
-      </c>
-      <c r="C91" s="20">
-        <v>-8.0410776736114098</v>
-      </c>
-      <c r="D91" s="20">
-        <v>-34.904317758007501</v>
+        <v>68</v>
+      </c>
+      <c r="C91">
+        <v>-8.0686411420000006</v>
+      </c>
+      <c r="D91">
+        <v>-34.880234899999998</v>
       </c>
       <c r="E91">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="F91">
         <v>3</v>
@@ -3038,19 +3029,19 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>221</v>
+        <v>41</v>
       </c>
       <c r="B92" t="s">
-        <v>222</v>
-      </c>
-      <c r="C92">
-        <v>-8.0565599999999993</v>
-      </c>
-      <c r="D92">
-        <v>-34.9</v>
+        <v>38</v>
+      </c>
+      <c r="C92" s="11">
+        <v>-8.0410776736114098</v>
+      </c>
+      <c r="D92" s="11">
+        <v>-34.904317758007501</v>
       </c>
       <c r="E92">
-        <v>114</v>
+        <v>98</v>
       </c>
       <c r="F92">
         <v>3</v>
@@ -3058,19 +3049,19 @@
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>95</v>
+        <v>223</v>
       </c>
       <c r="B93" t="s">
-        <v>112</v>
-      </c>
-      <c r="C93" s="20">
-        <v>-8.0267300000000006</v>
-      </c>
-      <c r="D93" s="20">
-        <v>-34.918700000000001</v>
+        <v>224</v>
+      </c>
+      <c r="C93">
+        <v>-8.0565599999999993</v>
+      </c>
+      <c r="D93">
+        <v>-34.9</v>
       </c>
       <c r="E93">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="F93">
         <v>3</v>
@@ -3078,19 +3069,19 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>30</v>
+        <v>97</v>
       </c>
       <c r="B94" t="s">
-        <v>31</v>
-      </c>
-      <c r="C94">
-        <v>-8.0945099999999996</v>
-      </c>
-      <c r="D94">
-        <v>-34.913899999999998</v>
+        <v>114</v>
+      </c>
+      <c r="C94" s="11">
+        <v>-8.0267300000000006</v>
+      </c>
+      <c r="D94" s="11">
+        <v>-34.918700000000001</v>
       </c>
       <c r="E94">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="F94">
         <v>3</v>
@@ -3098,19 +3089,19 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>96</v>
+        <v>32</v>
       </c>
       <c r="B95" t="s">
-        <v>111</v>
-      </c>
-      <c r="C95" s="20">
-        <v>-8.0209019323429107</v>
-      </c>
-      <c r="D95" s="20">
-        <v>-34.917366133765498</v>
+        <v>33</v>
+      </c>
+      <c r="C95">
+        <v>-8.0945099999999996</v>
+      </c>
+      <c r="D95">
+        <v>-34.913899999999998</v>
       </c>
       <c r="E95">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="F95">
         <v>3</v>
@@ -3118,19 +3109,19 @@
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>53</v>
+        <v>98</v>
       </c>
       <c r="B96" t="s">
-        <v>54</v>
-      </c>
-      <c r="C96" s="20">
-        <v>-8.0622754000000008</v>
-      </c>
-      <c r="D96" s="20">
-        <v>-34.885648099999997</v>
+        <v>113</v>
+      </c>
+      <c r="C96" s="11">
+        <v>-8.0209019323429107</v>
+      </c>
+      <c r="D96" s="11">
+        <v>-34.917366133765498</v>
       </c>
       <c r="E96">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F96">
         <v>3</v>
@@ -3138,19 +3129,19 @@
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="B97" t="s">
-        <v>51</v>
-      </c>
-      <c r="C97" s="20">
-        <v>-8.0725033140000004</v>
-      </c>
-      <c r="D97" s="20">
-        <v>-34.886144160000001</v>
+        <v>56</v>
+      </c>
+      <c r="C97" s="11">
+        <v>-8.0622754000000008</v>
+      </c>
+      <c r="D97" s="11">
+        <v>-34.885648099999997</v>
       </c>
       <c r="E97">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="F97">
         <v>3</v>
@@ -3158,19 +3149,19 @@
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>24</v>
+        <v>52</v>
       </c>
       <c r="B98" t="s">
-        <v>23</v>
-      </c>
-      <c r="C98" s="20">
-        <v>-8.0313872200619407</v>
-      </c>
-      <c r="D98" s="20">
-        <v>-34.924635268843282</v>
+        <v>53</v>
+      </c>
+      <c r="C98" s="11">
+        <v>-8.0725033140000004</v>
+      </c>
+      <c r="D98" s="11">
+        <v>-34.886144160000001</v>
       </c>
       <c r="E98">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="F98">
         <v>3</v>
@@ -3178,39 +3169,39 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>158</v>
+        <v>26</v>
       </c>
       <c r="B99" t="s">
-        <v>80</v>
-      </c>
-      <c r="C99" s="20">
-        <v>-8.0646199999999997</v>
-      </c>
-      <c r="D99" s="20">
-        <v>-34.872889999999998</v>
+        <v>25</v>
+      </c>
+      <c r="C99" s="11">
+        <v>-8.0313872200619407</v>
+      </c>
+      <c r="D99" s="11">
+        <v>-34.924635268843282</v>
       </c>
       <c r="E99">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F99">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B100" t="s">
-        <v>3</v>
-      </c>
-      <c r="C100" s="8">
-        <v>-8.0619899999999998</v>
-      </c>
-      <c r="D100" s="9">
-        <v>-34.871519999999997</v>
+        <v>82</v>
+      </c>
+      <c r="C100" s="11">
+        <v>-8.0646199999999997</v>
+      </c>
+      <c r="D100" s="11">
+        <v>-34.872889999999998</v>
       </c>
       <c r="E100">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F100">
         <v>1</v>
@@ -3218,79 +3209,79 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B101" t="s">
-        <v>161</v>
-      </c>
-      <c r="C101">
-        <v>-8.0191721076781093</v>
-      </c>
-      <c r="D101">
-        <v>-34.915538393356499</v>
+        <v>5</v>
+      </c>
+      <c r="C101" s="8">
+        <v>-8.0619899999999998</v>
+      </c>
+      <c r="D101" s="9">
+        <v>-34.871519999999997</v>
       </c>
       <c r="E101">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F101">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>93</v>
+        <v>162</v>
       </c>
       <c r="B102" t="s">
-        <v>28</v>
-      </c>
-      <c r="C102" s="22">
-        <v>-8.0305944</v>
-      </c>
-      <c r="D102" s="23">
-        <v>-34.915496099999999</v>
+        <v>163</v>
+      </c>
+      <c r="C102">
+        <v>-8.0191721076781093</v>
+      </c>
+      <c r="D102">
+        <v>-34.915538393356499</v>
       </c>
       <c r="E102">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F102">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="B103" t="s">
-        <v>75</v>
-      </c>
-      <c r="C103" s="20">
-        <v>-8.0613100000000006</v>
-      </c>
-      <c r="D103" s="20">
-        <v>-34.872509999999998</v>
+        <v>30</v>
+      </c>
+      <c r="C103" s="13">
+        <v>-8.0305944</v>
+      </c>
+      <c r="D103" s="14">
+        <v>-34.915496099999999</v>
       </c>
       <c r="E103">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F103">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="B104" t="s">
-        <v>59</v>
-      </c>
-      <c r="C104" s="21">
-        <v>-8090593</v>
-      </c>
-      <c r="D104">
-        <v>-34.884158999999997</v>
+        <v>77</v>
+      </c>
+      <c r="C104" s="11">
+        <v>-8.0613100000000006</v>
+      </c>
+      <c r="D104" s="11">
+        <v>-34.872509999999998</v>
       </c>
       <c r="E104">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F104">
         <v>1</v>
@@ -3298,19 +3289,19 @@
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B105" t="s">
-        <v>68</v>
-      </c>
-      <c r="C105" s="20">
-        <v>-8.0605799999999999</v>
-      </c>
-      <c r="D105" s="20">
-        <v>-34.878079999999997</v>
+        <v>61</v>
+      </c>
+      <c r="C105">
+        <v>-8.0896899999999992</v>
+      </c>
+      <c r="D105">
+        <v>-34.882640000000002</v>
       </c>
       <c r="E105">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F105">
         <v>1</v>
@@ -3318,19 +3309,19 @@
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="B106" t="s">
-        <v>56</v>
-      </c>
-      <c r="C106">
-        <v>-8.0618400000000001</v>
-      </c>
-      <c r="D106">
-        <v>-34.884700000000002</v>
+        <v>70</v>
+      </c>
+      <c r="C106" s="11">
+        <v>-8.0605799999999999</v>
+      </c>
+      <c r="D106" s="11">
+        <v>-34.878079999999997</v>
       </c>
       <c r="E106">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F106">
         <v>1</v>
@@ -3338,19 +3329,19 @@
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="B107" t="s">
-        <v>73</v>
-      </c>
-      <c r="C107" s="8">
-        <v>-8.0610499999999998</v>
-      </c>
-      <c r="D107" s="9">
-        <v>-34.872990000000001</v>
+        <v>58</v>
+      </c>
+      <c r="C107">
+        <v>-8.0618400000000001</v>
+      </c>
+      <c r="D107">
+        <v>-34.884700000000002</v>
       </c>
       <c r="E107">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F107">
         <v>1</v>
@@ -3358,39 +3349,39 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>162</v>
-      </c>
-      <c r="B108" s="12" t="s">
-        <v>162</v>
-      </c>
-      <c r="C108" s="12">
-        <v>-8.0506770000000003</v>
-      </c>
-      <c r="D108" s="12">
-        <v>-34.872959999999999</v>
+        <v>74</v>
+      </c>
+      <c r="B108" t="s">
+        <v>75</v>
+      </c>
+      <c r="C108" s="8">
+        <v>-8.0610499999999998</v>
+      </c>
+      <c r="D108" s="9">
+        <v>-34.872990000000001</v>
       </c>
       <c r="E108">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F108">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>163</v>
-      </c>
-      <c r="B109" s="12" t="s">
-        <v>163</v>
-      </c>
-      <c r="C109" s="12">
-        <v>-8.06386</v>
-      </c>
-      <c r="D109" s="12">
-        <v>-34.875390000000003</v>
+        <v>164</v>
+      </c>
+      <c r="B109" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="C109" s="15">
+        <v>-8.0506770000000003</v>
+      </c>
+      <c r="D109" s="15">
+        <v>-34.872959999999999</v>
       </c>
       <c r="E109">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F109">
         <v>2</v>
@@ -3398,19 +3389,19 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>164</v>
-      </c>
-      <c r="B110" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="C110" s="12">
-        <v>-8.0619700000000005</v>
-      </c>
-      <c r="D110" s="12">
-        <v>-34.875079999999997</v>
+        <v>165</v>
+      </c>
+      <c r="B110" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C110" s="15">
+        <v>-8.06386</v>
+      </c>
+      <c r="D110" s="15">
+        <v>-34.875390000000003</v>
       </c>
       <c r="E110">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F110">
         <v>2</v>
@@ -3418,19 +3409,19 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>165</v>
-      </c>
-      <c r="B111" s="12" t="s">
-        <v>165</v>
-      </c>
-      <c r="C111" s="12">
-        <v>-8.0671199999999992</v>
-      </c>
-      <c r="D111" s="12">
-        <v>-34.873989999999999</v>
+        <v>166</v>
+      </c>
+      <c r="B111" s="15" t="s">
+        <v>166</v>
+      </c>
+      <c r="C111" s="15">
+        <v>-8.0619700000000005</v>
+      </c>
+      <c r="D111" s="15">
+        <v>-34.875079999999997</v>
       </c>
       <c r="E111">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F111">
         <v>2</v>
@@ -3438,19 +3429,19 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>166</v>
-      </c>
-      <c r="B112" s="12" t="s">
-        <v>166</v>
-      </c>
-      <c r="C112" s="12">
-        <v>-8.05992</v>
-      </c>
-      <c r="D112" s="12">
-        <v>-34.879330000000003</v>
+        <v>167</v>
+      </c>
+      <c r="B112" s="15" t="s">
+        <v>167</v>
+      </c>
+      <c r="C112" s="15">
+        <v>-8.0671199999999992</v>
+      </c>
+      <c r="D112" s="15">
+        <v>-34.873989999999999</v>
       </c>
       <c r="E112">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F112">
         <v>2</v>
@@ -3458,19 +3449,19 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>167</v>
-      </c>
-      <c r="B113" s="12" t="s">
-        <v>167</v>
-      </c>
-      <c r="C113" s="12">
-        <v>-8.0623199999999997</v>
-      </c>
-      <c r="D113" s="12">
-        <v>-34.881039999999999</v>
+        <v>168</v>
+      </c>
+      <c r="B113" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="C113" s="15">
+        <v>-8.05992</v>
+      </c>
+      <c r="D113" s="15">
+        <v>-34.879330000000003</v>
       </c>
       <c r="E113">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F113">
         <v>2</v>
@@ -3478,19 +3469,19 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>168</v>
-      </c>
-      <c r="B114" s="12" t="s">
-        <v>168</v>
-      </c>
-      <c r="C114" s="12">
-        <v>-8.0659799999999997</v>
-      </c>
-      <c r="D114" s="12">
-        <v>-34.884689999999999</v>
+        <v>169</v>
+      </c>
+      <c r="B114" s="15" t="s">
+        <v>169</v>
+      </c>
+      <c r="C114" s="15">
+        <v>-8.0623199999999997</v>
+      </c>
+      <c r="D114" s="15">
+        <v>-34.881039999999999</v>
       </c>
       <c r="E114">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F114">
         <v>2</v>
@@ -3498,19 +3489,19 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>169</v>
-      </c>
-      <c r="B115" s="12" t="s">
-        <v>169</v>
-      </c>
-      <c r="C115" s="12">
-        <v>-8.045477</v>
-      </c>
-      <c r="D115" s="12">
-        <v>-8.045477</v>
+        <v>170</v>
+      </c>
+      <c r="B115" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="C115" s="15">
+        <v>-8.0659799999999997</v>
+      </c>
+      <c r="D115" s="15">
+        <v>-34.884689999999999</v>
       </c>
       <c r="E115">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F115">
         <v>2</v>
@@ -3518,19 +3509,19 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>170</v>
-      </c>
-      <c r="B116" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="C116" s="12">
-        <v>-8.0827240000000007</v>
-      </c>
-      <c r="D116" s="12">
-        <v>-34.890836999999998</v>
+        <v>171</v>
+      </c>
+      <c r="B116" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C116" s="15">
+        <v>-8.045477</v>
+      </c>
+      <c r="D116" s="15">
+        <v>-8.045477</v>
       </c>
       <c r="E116">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F116">
         <v>2</v>
@@ -3538,19 +3529,19 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>170</v>
-      </c>
-      <c r="B117" s="12" t="s">
-        <v>174</v>
-      </c>
-      <c r="C117" s="12">
-        <v>-8.0822699999999994</v>
-      </c>
-      <c r="D117" s="12">
-        <v>-34.889646999999997</v>
+        <v>172</v>
+      </c>
+      <c r="B117" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="C117" s="15">
+        <v>-8.0827240000000007</v>
+      </c>
+      <c r="D117" s="15">
+        <v>-34.890836999999998</v>
       </c>
       <c r="E117">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F117">
         <v>2</v>
@@ -3558,39 +3549,39 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>171</v>
-      </c>
-      <c r="B118" s="12" t="s">
-        <v>171</v>
-      </c>
-      <c r="C118" s="12">
-        <v>-8.0577939999999995</v>
-      </c>
-      <c r="D118" s="12">
-        <v>-34.909590999999999</v>
+        <v>172</v>
+      </c>
+      <c r="B118" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="C118" s="15">
+        <v>-8.0822699999999994</v>
+      </c>
+      <c r="D118" s="15">
+        <v>-34.889646999999997</v>
       </c>
       <c r="E118">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F118">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>118</v>
-      </c>
-      <c r="B119" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="C119" s="12">
-        <v>-8.0615539999999992</v>
-      </c>
-      <c r="D119" s="12">
-        <v>-34.901347999999999</v>
+        <v>173</v>
+      </c>
+      <c r="B119" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="C119" s="15">
+        <v>-8.0577939999999995</v>
+      </c>
+      <c r="D119" s="15">
+        <v>-34.909590999999999</v>
       </c>
       <c r="E119">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F119">
         <v>1</v>
@@ -3598,19 +3589,19 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>172</v>
-      </c>
-      <c r="B120" s="12" t="s">
-        <v>172</v>
-      </c>
-      <c r="C120" s="12">
-        <v>-8.0865039999999997</v>
-      </c>
-      <c r="D120" s="12">
-        <v>-34.888176000000001</v>
+        <v>120</v>
+      </c>
+      <c r="B120" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="C120" s="15">
+        <v>-8.0615539999999992</v>
+      </c>
+      <c r="D120" s="15">
+        <v>-34.901347999999999</v>
       </c>
       <c r="E120">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F120">
         <v>1</v>
@@ -3618,19 +3609,19 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>173</v>
-      </c>
-      <c r="B121" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C121" s="12">
-        <v>-8.1233310000000003</v>
-      </c>
-      <c r="D121" s="12">
-        <v>-34.909514999999999</v>
+        <v>174</v>
+      </c>
+      <c r="B121" s="15" t="s">
+        <v>174</v>
+      </c>
+      <c r="C121" s="15">
+        <v>-8.0865039999999997</v>
+      </c>
+      <c r="D121" s="15">
+        <v>-34.888176000000001</v>
       </c>
       <c r="E121">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F121">
         <v>1</v>
@@ -3638,19 +3629,19 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>173</v>
-      </c>
-      <c r="B122" s="12" t="s">
-        <v>173</v>
-      </c>
-      <c r="C122" s="12">
-        <v>-8.1232679999999995</v>
-      </c>
-      <c r="D122" s="12">
-        <v>-34.909429000000003</v>
+        <v>175</v>
+      </c>
+      <c r="B122" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="C122" s="15">
+        <v>-8.1233310000000003</v>
+      </c>
+      <c r="D122" s="15">
+        <v>-34.909514999999999</v>
       </c>
       <c r="E122">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F122">
         <v>1</v>
@@ -3660,336 +3651,255 @@
       <c r="A123" t="s">
         <v>175</v>
       </c>
-      <c r="B123" s="12" t="s">
+      <c r="B123" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="C123" s="14">
+      <c r="C123" s="15">
+        <v>-8.1232679999999995</v>
+      </c>
+      <c r="D123" s="15">
+        <v>-34.909429000000003</v>
+      </c>
+      <c r="E123">
+        <v>144</v>
+      </c>
+      <c r="F123">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A124" t="s">
+        <v>177</v>
+      </c>
+      <c r="B124" s="15" t="s">
+        <v>177</v>
+      </c>
+      <c r="C124" s="17">
         <v>-8.1048700733912096</v>
       </c>
-      <c r="D123" s="24">
+      <c r="D124" s="21">
         <v>-34.891163918022997</v>
       </c>
-      <c r="E123">
+      <c r="E124">
         <v>145</v>
       </c>
-      <c r="F123">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="124" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A124" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="B124" s="18" t="s">
-        <v>223</v>
-      </c>
-      <c r="C124" s="25">
+      <c r="F124">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="B125" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="C125" s="24">
         <v>-8.0635997672068793</v>
       </c>
-      <c r="D124" s="25">
+      <c r="D125" s="24">
         <v>-34.881890011734797</v>
       </c>
-      <c r="E124">
-        <v>146</v>
-      </c>
-      <c r="F124">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="125" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="B125" s="18" t="s">
-        <v>224</v>
-      </c>
-      <c r="C125" s="26">
+    </row>
+    <row r="126" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A126" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="B126" s="22" t="s">
+        <v>226</v>
+      </c>
+      <c r="C126" s="25">
         <v>-8.0297949481864208</v>
       </c>
-      <c r="D125" s="26">
+      <c r="D126" s="25">
         <v>-34.929545690228501</v>
       </c>
-      <c r="E125">
-        <v>147</v>
-      </c>
-      <c r="F125">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A126" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="B126" t="s">
-        <v>197</v>
-      </c>
-      <c r="C126" s="13">
-        <v>-8.1129139186695003</v>
-      </c>
-      <c r="D126" s="13">
-        <v>-34.892622764508502</v>
-      </c>
-      <c r="E126">
-        <v>148</v>
-      </c>
-      <c r="F126">
-        <v>1</v>
-      </c>
-      <c r="G126" t="s">
-        <v>176</v>
-      </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A127" t="s">
-        <v>185</v>
+      <c r="A127" s="5" t="s">
+        <v>179</v>
       </c>
       <c r="B127" t="s">
-        <v>198</v>
-      </c>
-      <c r="C127" s="14">
-        <v>-8.1213842543624306</v>
-      </c>
-      <c r="D127" s="14">
-        <v>-34.896742272749499</v>
-      </c>
-      <c r="E127">
-        <v>149</v>
-      </c>
-      <c r="F127">
-        <v>1</v>
+        <v>199</v>
+      </c>
+      <c r="C127" s="16">
+        <v>-8.1062248248406696</v>
+      </c>
+      <c r="D127" s="16">
+        <v>-34.889176660810698</v>
       </c>
       <c r="G127" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A128" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="B128" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="C128" s="14">
+      <c r="A128" t="s">
+        <v>187</v>
+      </c>
+      <c r="B128" t="s">
+        <v>200</v>
+      </c>
+      <c r="C128" s="17">
+        <v>-8.1213842543624306</v>
+      </c>
+      <c r="D128" s="17">
+        <v>-34.896742272749499</v>
+      </c>
+      <c r="G128" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A129" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="B129" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="C129" s="17">
         <v>-8.0951588190898107</v>
       </c>
-      <c r="D128" s="14">
+      <c r="D129" s="17">
         <v>-34.885862444833599</v>
       </c>
-      <c r="E128">
-        <v>150</v>
-      </c>
-      <c r="F128">
-        <v>2</v>
-      </c>
-      <c r="G128" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A129" t="s">
-        <v>184</v>
-      </c>
-      <c r="B129" t="s">
-        <v>199</v>
-      </c>
-      <c r="C129" s="13">
-        <v>-8.1234744929365093</v>
-      </c>
-      <c r="D129" s="13">
-        <v>-34.899869662926399</v>
-      </c>
-      <c r="E129">
-        <v>151</v>
-      </c>
-      <c r="F129">
-        <v>1</v>
-      </c>
       <c r="G129" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B130" t="s">
-        <v>200</v>
-      </c>
-      <c r="C130" s="15">
-        <v>-8.1316445036234501</v>
-      </c>
-      <c r="D130" s="15">
-        <v>-34.902758621825001</v>
-      </c>
-      <c r="E130">
-        <v>152</v>
-      </c>
-      <c r="F130">
-        <v>2</v>
+        <v>201</v>
+      </c>
+      <c r="C130" s="16">
+        <v>-8.1234744929365093</v>
+      </c>
+      <c r="D130" s="16">
+        <v>-34.899869662926399</v>
       </c>
       <c r="G130" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B131" t="s">
         <v>202</v>
       </c>
-      <c r="C131" s="15">
+      <c r="C131" s="18">
+        <v>-8.1316445036234501</v>
+      </c>
+      <c r="D131" s="18">
+        <v>-34.902758621825001</v>
+      </c>
+      <c r="G131" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A132" t="s">
+        <v>190</v>
+      </c>
+      <c r="B132" t="s">
+        <v>204</v>
+      </c>
+      <c r="C132" s="18">
         <v>-8.1443519397406607</v>
       </c>
-      <c r="D131" s="15">
+      <c r="D132" s="18">
         <v>-34.906480195132502</v>
       </c>
-      <c r="E131">
-        <v>153</v>
-      </c>
-      <c r="F131">
-        <v>1</v>
-      </c>
-      <c r="G131" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A132" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="B132" t="s">
-        <v>201</v>
-      </c>
-      <c r="C132" s="14">
+      <c r="G132" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A133" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="B133" t="s">
+        <v>203</v>
+      </c>
+      <c r="C133" s="17">
         <v>-8.1357574755544597</v>
       </c>
-      <c r="D132" s="14">
+      <c r="D133" s="17">
         <v>-34.908424559020403</v>
       </c>
-      <c r="E132">
-        <v>154</v>
-      </c>
-      <c r="F132">
-        <v>2</v>
-      </c>
-      <c r="G132" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A133" t="s">
-        <v>194</v>
-      </c>
-      <c r="B133" t="s">
-        <v>205</v>
-      </c>
-      <c r="C133" s="13">
-        <v>-8.0682650000000002</v>
-      </c>
-      <c r="D133" s="13">
-        <v>-34.909804999999999</v>
-      </c>
-      <c r="E133">
-        <v>155</v>
-      </c>
-      <c r="F133">
-        <v>1</v>
-      </c>
       <c r="G133" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
+        <v>196</v>
+      </c>
+      <c r="B134" t="s">
         <v>207</v>
       </c>
-      <c r="B134" t="s">
-        <v>206</v>
-      </c>
-      <c r="C134" s="13">
-        <v>-8.0577959999999997</v>
-      </c>
-      <c r="D134" s="13">
-        <v>-34.883166000000003</v>
-      </c>
-      <c r="E134">
-        <v>156</v>
-      </c>
-      <c r="F134">
-        <v>1</v>
+      <c r="C134" s="16">
+        <v>-8.0682650000000002</v>
+      </c>
+      <c r="D134" s="16">
+        <v>-34.909804999999999</v>
       </c>
       <c r="G134" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="B135" t="s">
         <v>208</v>
       </c>
-      <c r="C135" s="13">
+      <c r="C135" s="16">
+        <v>-8.0577959999999997</v>
+      </c>
+      <c r="D135" s="16">
+        <v>-34.883166000000003</v>
+      </c>
+      <c r="G135" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A136" t="s">
+        <v>197</v>
+      </c>
+      <c r="B136" t="s">
+        <v>210</v>
+      </c>
+      <c r="C136" s="16">
         <v>-8.0451259999999998</v>
       </c>
-      <c r="D135" s="13">
+      <c r="D136" s="16">
         <v>-34.902045999999999</v>
       </c>
-      <c r="E135">
-        <v>157</v>
-      </c>
-      <c r="F135">
-        <v>1</v>
-      </c>
-      <c r="G135" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A136" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="B136" s="18" t="s">
-        <v>210</v>
-      </c>
-      <c r="C136" s="13">
+      <c r="G136" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A137" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="B137" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="C137" s="16">
         <v>-8.0595918660612593</v>
       </c>
-      <c r="D136" s="13">
+      <c r="D137" s="16">
         <v>-34.886419614608201</v>
       </c>
-      <c r="E136">
-        <v>158</v>
-      </c>
-      <c r="F136">
-        <v>1</v>
-      </c>
-      <c r="G136" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A137" t="s">
-        <v>211</v>
-      </c>
-      <c r="B137" t="s">
-        <v>212</v>
-      </c>
-      <c r="C137" s="13">
-        <v>-8.0239212086655201</v>
-      </c>
-      <c r="D137" s="13">
-        <v>-34.897226975193099</v>
-      </c>
-      <c r="E137">
-        <v>159</v>
-      </c>
-      <c r="F137">
-        <v>1</v>
-      </c>
       <c r="G137" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
@@ -3999,103 +3909,79 @@
       <c r="B138" t="s">
         <v>214</v>
       </c>
-      <c r="C138" s="13">
-        <v>-8.0313044697048603</v>
-      </c>
-      <c r="D138" s="13">
-        <v>-34.902172963415303</v>
-      </c>
-      <c r="E138">
-        <v>160</v>
-      </c>
-      <c r="F138">
-        <v>1</v>
+      <c r="C138" s="16">
+        <v>-8.0239212086655201</v>
+      </c>
+      <c r="D138" s="16">
+        <v>-34.897226975193099</v>
       </c>
       <c r="G138" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
+        <v>215</v>
+      </c>
+      <c r="B139" t="s">
         <v>216</v>
       </c>
-      <c r="B139" t="s">
-        <v>215</v>
-      </c>
-      <c r="C139" s="13">
-        <v>-8.0990571360815995</v>
-      </c>
-      <c r="D139" s="13">
-        <v>-34.885838700681703</v>
-      </c>
-      <c r="E139">
-        <v>161</v>
-      </c>
-      <c r="F139">
-        <v>2</v>
+      <c r="C139" s="16">
+        <v>-8.0313044697048603</v>
+      </c>
+      <c r="D139" s="16">
+        <v>-34.902172963415303</v>
       </c>
       <c r="G139" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B140" t="s">
-        <v>220</v>
-      </c>
-      <c r="C140" s="13">
-        <v>-8.1162072256009594</v>
-      </c>
-      <c r="D140" s="13">
-        <v>-34.894632005796097</v>
-      </c>
-      <c r="E140">
-        <v>162</v>
-      </c>
-      <c r="F140">
-        <v>1</v>
+        <v>217</v>
+      </c>
+      <c r="C140" s="16">
+        <v>-8.0990571360815995</v>
+      </c>
+      <c r="D140" s="16">
+        <v>-34.885838700681703</v>
       </c>
       <c r="G140" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="B141" t="s">
-        <v>220</v>
-      </c>
-      <c r="C141" s="13">
+        <v>222</v>
+      </c>
+      <c r="C141" s="16">
         <v>-8.1162072256009594</v>
       </c>
-      <c r="D141" s="13">
+      <c r="D141" s="16">
         <v>-34.894632005796097</v>
       </c>
-      <c r="E141">
-        <v>163</v>
-      </c>
-      <c r="F141">
-        <v>1</v>
-      </c>
       <c r="G141" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D142" s="9"/>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C143" s="16"/>
+      <c r="C143" s="19"/>
       <c r="D143" s="9"/>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="D144" s="9"/>
     </row>
     <row r="145" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C145" s="17"/>
+      <c r="C145" s="20"/>
       <c r="D145" s="9"/>
     </row>
     <row r="146" spans="3:4" x14ac:dyDescent="0.3">
@@ -4108,7 +3994,7 @@
       <c r="D148" s="9"/>
     </row>
     <row r="149" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C149" s="16"/>
+      <c r="C149" s="19"/>
       <c r="D149" s="9"/>
     </row>
     <row r="150" spans="3:4" x14ac:dyDescent="0.3">
@@ -4118,21 +4004,21 @@
       <c r="D151" s="9"/>
     </row>
     <row r="152" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C152" s="16"/>
+      <c r="C152" s="19"/>
       <c r="D152" s="9"/>
     </row>
     <row r="153" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D153" s="9"/>
     </row>
     <row r="154" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C154" s="16"/>
+      <c r="C154" s="19"/>
       <c r="D154" s="9"/>
     </row>
     <row r="155" spans="3:4" x14ac:dyDescent="0.3">
       <c r="D155" s="9"/>
     </row>
     <row r="156" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C156" s="17"/>
+      <c r="C156" s="20"/>
       <c r="D156" s="9"/>
     </row>
     <row r="157" spans="3:4" x14ac:dyDescent="0.3">
@@ -4166,11 +4052,11 @@
       <c r="D166" s="9"/>
     </row>
     <row r="167" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C167" s="17"/>
+      <c r="C167" s="20"/>
       <c r="D167" s="9"/>
     </row>
     <row r="168" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C168" s="17"/>
+      <c r="C168" s="20"/>
       <c r="D168" s="9"/>
     </row>
     <row r="169" spans="3:4" x14ac:dyDescent="0.3">
@@ -4601,7 +4487,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:F141" xr:uid="{22014C47-1C13-4AB1-9850-A592523522E1}"/>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
@@ -4624,191 +4510,191 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="C1" t="s">
-        <v>204</v>
+        <v>206</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C2" t="s">
-        <v>197</v>
-      </c>
-      <c r="D2" s="13">
+        <v>199</v>
+      </c>
+      <c r="D2" s="16">
         <v>-8.1062248248406696</v>
       </c>
-      <c r="E2" s="13">
+      <c r="E2" s="16">
         <v>-34.889176660810698</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="C3" t="s">
-        <v>198</v>
-      </c>
-      <c r="D3" s="14">
+        <v>200</v>
+      </c>
+      <c r="D3" s="17">
         <v>-8.1213842543624306</v>
       </c>
-      <c r="E3" s="14">
+      <c r="E3" s="17">
         <v>-34.896742272749499</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>179</v>
-      </c>
-      <c r="B4" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="D4" s="14">
+        <v>181</v>
+      </c>
+      <c r="B4" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="C4" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="D4" s="17">
         <v>-8095158819089810</v>
       </c>
-      <c r="E4" s="14" t="s">
-        <v>218</v>
+      <c r="E4" s="17" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="B5" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C5" t="s">
-        <v>199</v>
-      </c>
-      <c r="D5" s="13">
+        <v>201</v>
+      </c>
+      <c r="D5" s="16">
         <v>-8.1234744929365093</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="16">
         <v>-34.899869662926399</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="B6" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="C6" t="s">
-        <v>200</v>
-      </c>
-      <c r="D6" s="15">
+        <v>202</v>
+      </c>
+      <c r="D6" s="18">
         <v>-8131644503623450</v>
       </c>
-      <c r="E6" s="15">
+      <c r="E6" s="18">
         <v>-3490275862182500</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="B7" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C7" t="s">
-        <v>202</v>
-      </c>
-      <c r="D7" s="15">
+        <v>204</v>
+      </c>
+      <c r="D7" s="18">
         <v>-8.1443519397406607</v>
       </c>
-      <c r="E7" s="15">
+      <c r="E7" s="18">
         <v>-34.906480195132502</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>189</v>
+        <v>191</v>
       </c>
       <c r="C8" t="s">
-        <v>201</v>
-      </c>
-      <c r="D8" s="14">
+        <v>203</v>
+      </c>
+      <c r="D8" s="17">
         <v>-8.1357574755544597</v>
       </c>
-      <c r="E8" s="14">
+      <c r="E8" s="17">
         <v>-34.908424559020403</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>186</v>
+        <v>188</v>
       </c>
       <c r="B9" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
       <c r="C9" t="s">
-        <v>205</v>
-      </c>
-      <c r="D9" s="13">
+        <v>207</v>
+      </c>
+      <c r="D9" s="16">
         <v>-8.0682650000000002</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="16">
         <v>-34.909804999999999</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="B10" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C10" t="s">
-        <v>206</v>
-      </c>
-      <c r="D10" s="13">
+        <v>208</v>
+      </c>
+      <c r="D10" s="16">
         <v>-8.0577959999999997</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E10" s="16">
         <v>-34.883166000000003</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="B11" t="s">
-        <v>195</v>
+        <v>197</v>
       </c>
       <c r="C11" t="s">
-        <v>208</v>
-      </c>
-      <c r="D11" s="13">
+        <v>210</v>
+      </c>
+      <c r="D11" s="16">
         <v>-8.0451259999999998</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="16">
         <v>-34.902045999999999</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>191</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>209</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>210</v>
+        <v>193</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="C12" s="22" t="s">
+        <v>212</v>
       </c>
       <c r="D12" s="1">
         <v>-8059591866061260</v>
@@ -4819,13 +4705,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="B13" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C13" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="D13" s="1">
         <v>-8023921208665520</v>
@@ -4836,13 +4722,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B14" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C14" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="D14" s="1">
         <v>-8031304469704860</v>
@@ -4853,13 +4739,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="B15" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C15" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="D15" s="1">
         <v>-8099057136081600</v>
@@ -4870,13 +4756,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>219</v>
+        <v>221</v>
       </c>
       <c r="B16" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C16" t="s">
-        <v>220</v>
+        <v>222</v>
       </c>
       <c r="D16" s="1">
         <v>-8116207225600960</v>
@@ -4892,7 +4778,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajustando detalhamento dos pontos mínimos.
</commit_message>
<xml_diff>
--- a/data/Prioridades.xlsx
+++ b/data/Prioridades.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Consultor\OneDrive - Aquila\Área de Trabalho\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Consultor\Desktop\COP\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEB63FC9-04B2-4E88-B73C-3D2D151043DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B29662D3-65A2-47D2-92AC-C0117D8AA673}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{397ABB56-F0FE-4E29-B5CB-823307B18FC8}"/>
   </bookViews>
@@ -379,9 +379,6 @@
     <t>LARGO DE CASA AMARELA</t>
   </si>
   <si>
-    <t>NOME</t>
-  </si>
-  <si>
     <t>LOGRADOURO</t>
   </si>
   <si>
@@ -719,6 +716,9 @@
   </si>
   <si>
     <t>LONGITUDE COM PONTO</t>
+  </si>
+  <si>
+    <t>TIPO</t>
   </si>
 </sst>
 </file>
@@ -1203,7 +1203,7 @@
   <dimension ref="A1:G676"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1218,30 +1218,30 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1" t="s">
         <v>113</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D1" t="s">
+        <v>225</v>
+      </c>
+      <c r="E1" t="s">
         <v>114</v>
       </c>
-      <c r="C1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D1" t="s">
-        <v>226</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>115</v>
-      </c>
-      <c r="F1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C2" s="13">
         <v>-8.0625199999999992</v>
@@ -1258,10 +1258,10 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C3" s="13">
         <v>-8.0349699999999995</v>
@@ -1278,10 +1278,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C4" s="13">
         <v>-8.0387400000000007</v>
@@ -1298,10 +1298,10 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C5" s="13">
         <v>-8.0782500000000006</v>
@@ -1318,10 +1318,10 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C6" s="13">
         <v>-8.0895499999999991</v>
@@ -1338,10 +1338,10 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C7" s="13">
         <v>-8.11951</v>
@@ -1358,10 +1358,10 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C8" s="13">
         <v>-8.0474399999999999</v>
@@ -1378,10 +1378,10 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C9" s="13">
         <v>-8.0848800000000001</v>
@@ -1398,10 +1398,10 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C10" s="13">
         <v>-8.1367899999999995</v>
@@ -1418,10 +1418,10 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B11" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C11" s="13">
         <v>-8.1222300000000001</v>
@@ -1438,10 +1438,10 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C12" s="13">
         <v>-8.1186299999999996</v>
@@ -1458,10 +1458,10 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C13" s="13">
         <v>-8.1115499999999994</v>
@@ -1478,10 +1478,10 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C14" s="13">
         <v>-8.1089400000000005</v>
@@ -1498,10 +1498,10 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C15" s="13">
         <v>-8.1061999999999994</v>
@@ -1518,10 +1518,10 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C16" s="13">
         <v>-8.0472400000000004</v>
@@ -1538,10 +1538,10 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B17" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C17" s="13">
         <v>-8.0501900000000006</v>
@@ -1558,10 +1558,10 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B18" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C18" s="13">
         <v>-8.0502800000000008</v>
@@ -1578,10 +1578,10 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B19" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C19" s="13">
         <v>-8.0542800000000003</v>
@@ -1598,10 +1598,10 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C20" s="13">
         <v>-8.0571900000000003</v>
@@ -1618,10 +1618,10 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C21" s="13">
         <v>-8.0796600000000005</v>
@@ -1638,10 +1638,10 @@
     </row>
     <row r="22" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C22" s="13">
         <v>-8.1066699999999994</v>
@@ -1658,10 +1658,10 @@
     </row>
     <row r="23" spans="1:6" s="7" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C23" s="13">
         <v>-8.1077700000000004</v>
@@ -1678,10 +1678,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C24" s="13">
         <v>-8.0779700000000005</v>
@@ -1698,10 +1698,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C25" s="13">
         <v>-8.0017399999999999</v>
@@ -1718,10 +1718,10 @@
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C26" s="13">
         <v>-8.0254999999999992</v>
@@ -1738,10 +1738,10 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27" t="s">
         <v>126</v>
-      </c>
-      <c r="B27" t="s">
-        <v>127</v>
       </c>
       <c r="C27" s="13">
         <v>-8.0549599999999995</v>
@@ -1758,10 +1758,10 @@
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C28" s="13">
         <v>-8.0661900000000006</v>
@@ -1778,10 +1778,10 @@
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B29" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C29" s="13">
         <v>-8.0796600000000005</v>
@@ -1798,10 +1798,10 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B30" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C30" s="13">
         <v>-8.0782000000000007</v>
@@ -1818,10 +1818,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C31" s="13">
         <v>-8.1105800000000006</v>
@@ -1838,10 +1838,10 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C32" s="13">
         <v>-8.1229300000000002</v>
@@ -1858,10 +1858,10 @@
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B33" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C33" s="13">
         <v>-8.1418700000000008</v>
@@ -1878,7 +1878,7 @@
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B34" t="s">
         <v>79</v>
@@ -1898,10 +1898,10 @@
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
+        <v>141</v>
+      </c>
+      <c r="B35" t="s">
         <v>142</v>
-      </c>
-      <c r="B35" t="s">
-        <v>143</v>
       </c>
       <c r="C35" s="13">
         <v>-8.0658437972273997</v>
@@ -1918,7 +1918,7 @@
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B36" t="s">
         <v>82</v>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="11" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B37" t="s">
         <v>57</v>
@@ -1978,7 +1978,7 @@
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B39" t="s">
         <v>77</v>
@@ -2101,7 +2101,7 @@
         <v>86</v>
       </c>
       <c r="B45" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C45" s="13">
         <v>-8.0774484770977697</v>
@@ -2258,7 +2258,7 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B53" t="s">
         <v>40</v>
@@ -2278,7 +2278,7 @@
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B54" t="s">
         <v>105</v>
@@ -2298,7 +2298,7 @@
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B55" t="s">
         <v>81</v>
@@ -2318,10 +2318,10 @@
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>149</v>
+      </c>
+      <c r="B56" t="s">
         <v>150</v>
-      </c>
-      <c r="B56" t="s">
-        <v>151</v>
       </c>
       <c r="C56" s="13">
         <v>-8.0933499999999992</v>
@@ -2458,7 +2458,7 @@
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B63" t="s">
         <v>83</v>
@@ -2478,10 +2478,10 @@
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>152</v>
+      </c>
+      <c r="B64" s="5" t="s">
         <v>153</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>154</v>
       </c>
       <c r="C64" s="13">
         <v>-8.0757700000000003</v>
@@ -2498,10 +2498,10 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
+        <v>154</v>
+      </c>
+      <c r="B65" t="s">
         <v>155</v>
-      </c>
-      <c r="B65" t="s">
-        <v>156</v>
       </c>
       <c r="C65" s="13">
         <v>-8.0682399999999994</v>
@@ -2978,7 +2978,7 @@
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B89" t="s">
         <v>17</v>
@@ -3038,10 +3038,10 @@
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
+        <v>220</v>
+      </c>
+      <c r="B92" t="s">
         <v>221</v>
-      </c>
-      <c r="B92" t="s">
-        <v>222</v>
       </c>
       <c r="C92">
         <v>-8.0565599999999993</v>
@@ -3178,7 +3178,7 @@
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B99" t="s">
         <v>80</v>
@@ -3198,7 +3198,7 @@
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B100" t="s">
         <v>3</v>
@@ -3218,10 +3218,10 @@
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
+        <v>159</v>
+      </c>
+      <c r="B101" t="s">
         <v>160</v>
-      </c>
-      <c r="B101" t="s">
-        <v>161</v>
       </c>
       <c r="C101">
         <v>-8.0191721076781093</v>
@@ -3358,10 +3358,10 @@
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B108" s="12" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C108" s="12">
         <v>-8.0506770000000003</v>
@@ -3378,10 +3378,10 @@
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B109" s="12" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C109" s="12">
         <v>-8.06386</v>
@@ -3398,10 +3398,10 @@
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B110" s="12" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C110" s="12">
         <v>-8.0619700000000005</v>
@@ -3418,10 +3418,10 @@
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B111" s="12" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C111" s="12">
         <v>-8.0671199999999992</v>
@@ -3438,10 +3438,10 @@
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B112" s="12" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C112" s="12">
         <v>-8.05992</v>
@@ -3458,10 +3458,10 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B113" s="12" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C113" s="12">
         <v>-8.0623199999999997</v>
@@ -3478,10 +3478,10 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B114" s="12" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C114" s="12">
         <v>-8.0659799999999997</v>
@@ -3498,10 +3498,10 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B115" s="12" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C115" s="12">
         <v>-8.045477</v>
@@ -3518,10 +3518,10 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B116" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C116" s="12">
         <v>-8.0827240000000007</v>
@@ -3538,10 +3538,10 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B117" s="12" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C117" s="12">
         <v>-8.0822699999999994</v>
@@ -3558,10 +3558,10 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B118" s="12" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C118" s="12">
         <v>-8.0577939999999995</v>
@@ -3578,10 +3578,10 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B119" s="12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C119" s="12">
         <v>-8.0615539999999992</v>
@@ -3598,10 +3598,10 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B120" s="12" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C120" s="12">
         <v>-8.0865039999999997</v>
@@ -3618,10 +3618,10 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B121" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C121" s="12">
         <v>-8.1233310000000003</v>
@@ -3638,10 +3638,10 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B122" s="12" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C122" s="12">
         <v>-8.1232679999999995</v>
@@ -3658,10 +3658,10 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B123" s="12" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C123" s="14">
         <v>-8.1048700733912096</v>
@@ -3678,10 +3678,10 @@
     </row>
     <row r="124" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A124" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B124" s="18" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C124" s="25">
         <v>-8.0635997672068793</v>
@@ -3698,10 +3698,10 @@
     </row>
     <row r="125" spans="1:7" s="18" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A125" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B125" s="18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C125" s="26">
         <v>-8.0297949481864208</v>
@@ -3718,10 +3718,10 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="5" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B126" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C126" s="13">
         <v>-8.1129139186695003</v>
@@ -3736,15 +3736,15 @@
         <v>1</v>
       </c>
       <c r="G126" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B127" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C127" s="14">
         <v>-8.1213842543624306</v>
@@ -3759,15 +3759,15 @@
         <v>1</v>
       </c>
       <c r="G127" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B128" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C128" s="14">
         <v>-8.0951588190898107</v>
@@ -3782,15 +3782,15 @@
         <v>2</v>
       </c>
       <c r="G128" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B129" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C129" s="13">
         <v>-8.1234744929365093</v>
@@ -3805,15 +3805,15 @@
         <v>1</v>
       </c>
       <c r="G129" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B130" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C130" s="15">
         <v>-8.1316445036234501</v>
@@ -3828,15 +3828,15 @@
         <v>2</v>
       </c>
       <c r="G130" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B131" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C131" s="15">
         <v>-8.1443519397406607</v>
@@ -3851,15 +3851,15 @@
         <v>1</v>
       </c>
       <c r="G131" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B132" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C132" s="14">
         <v>-8.1357574755544597</v>
@@ -3874,15 +3874,15 @@
         <v>2</v>
       </c>
       <c r="G132" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B133" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C133" s="13">
         <v>-8.0682650000000002</v>
@@ -3897,15 +3897,15 @@
         <v>1</v>
       </c>
       <c r="G133" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B134" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C134" s="13">
         <v>-8.0577959999999997</v>
@@ -3920,15 +3920,15 @@
         <v>1</v>
       </c>
       <c r="G134" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B135" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C135" s="13">
         <v>-8.0451259999999998</v>
@@ -3943,15 +3943,15 @@
         <v>1</v>
       </c>
       <c r="G135" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A136" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="B136" s="18" t="s">
         <v>209</v>
-      </c>
-      <c r="B136" s="18" t="s">
-        <v>210</v>
       </c>
       <c r="C136" s="13">
         <v>-8.0595918660612593</v>
@@ -3966,15 +3966,15 @@
         <v>1</v>
       </c>
       <c r="G136" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
+        <v>210</v>
+      </c>
+      <c r="B137" t="s">
         <v>211</v>
-      </c>
-      <c r="B137" t="s">
-        <v>212</v>
       </c>
       <c r="C137" s="13">
         <v>-8.0239212086655201</v>
@@ -3989,15 +3989,15 @@
         <v>1</v>
       </c>
       <c r="G137" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
+        <v>212</v>
+      </c>
+      <c r="B138" t="s">
         <v>213</v>
-      </c>
-      <c r="B138" t="s">
-        <v>214</v>
       </c>
       <c r="C138" s="13">
         <v>-8.0313044697048603</v>
@@ -4012,15 +4012,15 @@
         <v>1</v>
       </c>
       <c r="G138" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B139" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C139" s="13">
         <v>-8.0990571360815995</v>
@@ -4035,15 +4035,15 @@
         <v>2</v>
       </c>
       <c r="G139" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B140" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C140" s="13">
         <v>-8.1162072256009594</v>
@@ -4058,15 +4058,15 @@
         <v>1</v>
       </c>
       <c r="G140" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B141" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C141" s="13">
         <v>-8.1162072256009594</v>
@@ -4081,7 +4081,7 @@
         <v>1</v>
       </c>
       <c r="G141" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.3">
@@ -4624,21 +4624,21 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1" t="s">
         <v>203</v>
-      </c>
-      <c r="C1" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>175</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>176</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>177</v>
-      </c>
       <c r="C2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D2" s="13">
         <v>-8.1062248248406696</v>
@@ -4649,13 +4649,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D3" s="14">
         <v>-8.1213842543624306</v>
@@ -4666,30 +4666,30 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D4" s="14">
         <v>-8095158819089810</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D5" s="13">
         <v>-8.1234744929365093</v>
@@ -4700,13 +4700,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B6" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C6" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D6" s="15">
         <v>-8131644503623450</v>
@@ -4717,13 +4717,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D7" s="15">
         <v>-8.1443519397406607</v>
@@ -4734,13 +4734,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D8" s="14">
         <v>-8.1357574755544597</v>
@@ -4751,13 +4751,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B9" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C9" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D9" s="13">
         <v>-8.0682650000000002</v>
@@ -4768,13 +4768,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B10" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D10" s="13">
         <v>-8.0577959999999997</v>
@@ -4785,13 +4785,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D11" s="13">
         <v>-8.0451259999999998</v>
@@ -4802,13 +4802,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B12" s="18" t="s">
+        <v>208</v>
+      </c>
+      <c r="C12" s="18" t="s">
         <v>209</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>210</v>
       </c>
       <c r="D12" s="1">
         <v>-8059591866061260</v>
@@ -4819,13 +4819,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B13" t="s">
+        <v>210</v>
+      </c>
+      <c r="C13" t="s">
         <v>211</v>
-      </c>
-      <c r="C13" t="s">
-        <v>212</v>
       </c>
       <c r="D13" s="1">
         <v>-8023921208665520</v>
@@ -4836,13 +4836,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B14" t="s">
+        <v>212</v>
+      </c>
+      <c r="C14" t="s">
         <v>213</v>
-      </c>
-      <c r="C14" t="s">
-        <v>214</v>
       </c>
       <c r="D14" s="1">
         <v>-8031304469704860</v>
@@ -4853,13 +4853,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D15" s="1">
         <v>-8099057136081600</v>
@@ -4870,13 +4870,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
+        <v>218</v>
+      </c>
+      <c r="B16" t="s">
+        <v>215</v>
+      </c>
+      <c r="C16" t="s">
         <v>219</v>
-      </c>
-      <c r="B16" t="s">
-        <v>216</v>
-      </c>
-      <c r="C16" t="s">
-        <v>220</v>
       </c>
       <c r="D16" s="1">
         <v>-8116207225600960</v>

</xml_diff>